<commit_message>
GDE-6429 added condition on writing and fixed minor script issue
Delete rows on data set
</commit_message>
<xml_diff>
--- a/DataSet/LoanIQ_DataSet/EU_Entity/EVG_S1_EU_RPA_InternalDeal.xlsx
+++ b/DataSet/LoanIQ_DataSet/EU_Entity/EVG_S1_EU_RPA_InternalDeal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\LoanIQ_DataSet\EU_Entity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0570BAA-CB4D-41F5-95CE-5078B5843159}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A232FADB-73F7-4689-B471-BC1B4E89A8DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="923" firstSheet="10" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33630" yWindow="390" windowWidth="21600" windowHeight="11385" tabRatio="923" firstSheet="10" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PTY001_QuickPartyOnboarding" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1650" uniqueCount="865">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1644" uniqueCount="865">
   <si>
     <t>rowid</t>
   </si>
@@ -5255,10 +5255,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5373,37 +5373,6 @@
       </c>
       <c r="O2" s="88" t="s">
         <v>573</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="86" t="s">
-        <v>394</v>
-      </c>
-      <c r="B3" s="86"/>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86" t="s">
-        <v>551</v>
-      </c>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" t="s">
-        <v>551</v>
-      </c>
-      <c r="K3" s="90"/>
-      <c r="M3" s="91"/>
-    </row>
-    <row r="4" spans="1:15" s="86" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="86" t="s">
-        <v>553</v>
-      </c>
-      <c r="D4" t="s">
-        <v>554</v>
-      </c>
-      <c r="J4" t="s">
-        <v>554</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GDE-7566 - Removing Entity Tab in the Datasets
</commit_message>
<xml_diff>
--- a/DataSet/LoanIQ_DataSet/EU_Entity/EVG_S1_EU_RPA_InternalDeal.xlsx
+++ b/DataSet/LoanIQ_DataSet/EU_Entity/EVG_S1_EU_RPA_InternalDeal.xlsx
@@ -8,26 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\LoanIQ_DataSet\EU_Entity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593F3327-81F1-4BCB-AA6F-F2C9FFE5E0A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A232FADB-73F7-4689-B471-BC1B4E89A8DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="12885" firstSheet="12" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33630" yWindow="390" windowWidth="21600" windowHeight="11385" tabRatio="923" firstSheet="10" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PTY001_QuickPartyOnboarding" sheetId="1" r:id="rId1"/>
     <sheet name="Users_Fields" sheetId="2" r:id="rId2"/>
     <sheet name="ORIG03_Customer" sheetId="3" r:id="rId3"/>
     <sheet name="CRED01_DealSetup" sheetId="4" r:id="rId4"/>
-    <sheet name="CRED07_UpfrontFeeSetup" sheetId="5" r:id="rId5"/>
-    <sheet name="CRED02_FacilitySetup" sheetId="6" r:id="rId6"/>
-    <sheet name="CRED08_OngoingFeeSetup" sheetId="7" r:id="rId7"/>
-    <sheet name="SYND02_PrimaryAllocation" sheetId="8" r:id="rId8"/>
-    <sheet name="SERV01_LoanDrawdown" sheetId="9" r:id="rId9"/>
-    <sheet name="AMCH06_PricingChangeTransaction" sheetId="10" r:id="rId10"/>
-    <sheet name="DLCH01_DealChangeTransaction" sheetId="11" r:id="rId11"/>
-    <sheet name="SERV18_Payments" sheetId="12" r:id="rId12"/>
-    <sheet name="SERV21_InterestPayments" sheetId="13" r:id="rId13"/>
-    <sheet name="SERV29_PaymentFees" sheetId="14" r:id="rId14"/>
-    <sheet name="AMCH04_DealChangeTransaction" sheetId="15" r:id="rId15"/>
+    <sheet name="CRED07_UpfrontFeeSetup" sheetId="6" r:id="rId5"/>
+    <sheet name="CRED02_FacilitySetup" sheetId="7" r:id="rId6"/>
+    <sheet name="CRED08_OngoingFeeSetup" sheetId="8" r:id="rId7"/>
+    <sheet name="SYND02_PrimaryAllocation" sheetId="9" r:id="rId8"/>
+    <sheet name="SERV01_LoanDrawdown" sheetId="10" r:id="rId9"/>
+    <sheet name="AMCH06_PricingChangeTransaction" sheetId="11" r:id="rId10"/>
+    <sheet name="DLCH01_DealChangeTransaction" sheetId="12" r:id="rId11"/>
+    <sheet name="SERV18_Payments" sheetId="13" r:id="rId12"/>
+    <sheet name="SERV21_InterestPayments" sheetId="14" r:id="rId13"/>
+    <sheet name="SERV29_PaymentFees" sheetId="15" r:id="rId14"/>
+    <sheet name="AMCH04_DealChangeTransaction" sheetId="16" r:id="rId15"/>
+    <sheet name="TRPO12_PortfolioSettledDisc" sheetId="5" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1651" uniqueCount="847">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1644" uniqueCount="865">
   <si>
     <t>rowid</t>
   </si>
@@ -1594,13 +1595,13 @@
     <t>R1_</t>
   </si>
   <si>
-    <t>RPA INTERNAL 100M EURO19072020171734BVP</t>
-  </si>
-  <si>
-    <t>R1_19072020171737KCK</t>
-  </si>
-  <si>
-    <t>INTFULDRAW19072020175128ZRS</t>
+    <t>RPA INTERNAL 100M EURO13102020142627ZNK</t>
+  </si>
+  <si>
+    <t>R1_13102020142630ZCT</t>
+  </si>
+  <si>
+    <t>INTFULDRAW13102020151942AWM</t>
   </si>
   <si>
     <t>Sales Group 1</t>
@@ -1645,70 +1646,130 @@
     <t>1.00000000000</t>
   </si>
   <si>
+    <t>22-May-2020</t>
+  </si>
+  <si>
+    <t>Euro LIBOR Option</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>Modified Following Business Day</t>
+  </si>
+  <si>
+    <t>Next repricing date</t>
+  </si>
+  <si>
+    <t>Start of next interest cycle</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>12pm</t>
+  </si>
+  <si>
+    <t>OFF</t>
+  </si>
+  <si>
+    <t>Commitment Fee</t>
+  </si>
+  <si>
+    <t>Effective date of change</t>
+  </si>
+  <si>
+    <t>JONES</t>
+  </si>
+  <si>
+    <t>JONES,  JUGHEAD</t>
+  </si>
+  <si>
+    <t>Commonwealth Bank of Australia - Amsterdam</t>
+  </si>
+  <si>
+    <t>Team Amsterdam</t>
+  </si>
+  <si>
+    <t>Upfront Fee</t>
+  </si>
+  <si>
+    <t>Establishment/Extension Fee</t>
+  </si>
+  <si>
+    <t>Actual/360</t>
+  </si>
+  <si>
+    <t>5,000</t>
+  </si>
+  <si>
+    <t>PARDRAW13102020153004MDO</t>
+  </si>
+  <si>
     <t>27-May-2020</t>
   </si>
   <si>
-    <t>Euro LIBOR Option</t>
-  </si>
-  <si>
-    <t>Actual</t>
-  </si>
-  <si>
-    <t>Modified Following Business Day</t>
-  </si>
-  <si>
-    <t>Next repricing date</t>
-  </si>
-  <si>
-    <t>Start of next interest cycle</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>12pm</t>
-  </si>
-  <si>
-    <t>OFF</t>
-  </si>
-  <si>
-    <t>Commitment Fee</t>
-  </si>
-  <si>
-    <t>Effective date of change</t>
-  </si>
-  <si>
-    <t>JONES</t>
-  </si>
-  <si>
-    <t>JONES,  JUGHEAD</t>
-  </si>
-  <si>
-    <t>Commonwealth Bank of Australia - Amsterdam</t>
-  </si>
-  <si>
-    <t>Team Amsterdam</t>
-  </si>
-  <si>
-    <t>Upfront Fee</t>
-  </si>
-  <si>
-    <t>Establishment/Extension Fee</t>
-  </si>
-  <si>
-    <t>Actual/360</t>
-  </si>
-  <si>
-    <t>5,000</t>
-  </si>
-  <si>
-    <t>PARDRAW19072020180431GZX</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
-    <t>INTUND19072020181758HRH</t>
+    <t>INTUND13102020153805LRW</t>
+  </si>
+  <si>
+    <t>Short_Name</t>
+  </si>
+  <si>
+    <t>Transaction_Type</t>
+  </si>
+  <si>
+    <t>Transaction_Status_Awaiting_Approval</t>
+  </si>
+  <si>
+    <t>Payment_Type</t>
+  </si>
+  <si>
+    <t>Transaction_Status_Awaiting_Release</t>
+  </si>
+  <si>
+    <t>Portfolio_Position</t>
+  </si>
+  <si>
+    <t>Adjustment_Amount</t>
+  </si>
+  <si>
+    <t>GL_ShortName</t>
+  </si>
+  <si>
+    <t>AwaitingDispose</t>
+  </si>
+  <si>
+    <t>PFDC_Transaction_Type</t>
+  </si>
+  <si>
+    <t>PFDC_Payment_Type</t>
+  </si>
+  <si>
+    <t>Payments</t>
+  </si>
+  <si>
+    <t>Awaiting Approval</t>
+  </si>
+  <si>
+    <t>Fee Payment From Borrower</t>
+  </si>
+  <si>
+    <t>Awaiting Release</t>
+  </si>
+  <si>
+    <t>Interest Income</t>
+  </si>
+  <si>
+    <t>BNS1_02052020132235LFZ</t>
+  </si>
+  <si>
+    <t>Facilities</t>
+  </si>
+  <si>
+    <t>Portfolio Settled Discount Adjustment</t>
   </si>
   <si>
     <t>UpfrontFee_CategoryType</t>
@@ -1816,306 +1877,309 @@
     <t>50,000,000.00</t>
   </si>
   <si>
+    <t>21-May-2025</t>
+  </si>
+  <si>
+    <t>Fixed Rate Loan</t>
+  </si>
+  <si>
+    <t>FLOAT</t>
+  </si>
+  <si>
+    <t>Working Capital</t>
+  </si>
+  <si>
+    <t>100.000000%</t>
+  </si>
+  <si>
+    <t>Facility B Partially Drawn</t>
+  </si>
+  <si>
+    <t>PARDRAW</t>
+  </si>
+  <si>
+    <t>Revolver</t>
+  </si>
+  <si>
+    <t>30,000,000.00</t>
+  </si>
+  <si>
+    <t>Loan</t>
+  </si>
+  <si>
+    <t>Facility Internal Undrawn</t>
+  </si>
+  <si>
+    <t>INTUND</t>
+  </si>
+  <si>
+    <t>20,000,000.00</t>
+  </si>
+  <si>
+    <t>OngoingFee_Category1</t>
+  </si>
+  <si>
+    <t>OngoingFee_Type1</t>
+  </si>
+  <si>
+    <t>OngoingFee_RateBasis1</t>
+  </si>
+  <si>
+    <t>OngoingFee_AfterItem</t>
+  </si>
+  <si>
+    <t>OngoingFee_AfterItemType</t>
+  </si>
+  <si>
+    <t>Facility_PercentWhole</t>
+  </si>
+  <si>
+    <t>Facility_Percent</t>
+  </si>
+  <si>
+    <t>OngoingFee_SpreadType1</t>
+  </si>
+  <si>
+    <t>OngoingFee_SpreadType2</t>
+  </si>
+  <si>
+    <t>Interest_AddItem</t>
+  </si>
+  <si>
+    <t>Interest_OptionName1</t>
+  </si>
+  <si>
+    <t>Interest_RateBasis</t>
+  </si>
+  <si>
+    <t>Interest_SpreadType1</t>
+  </si>
+  <si>
+    <t>Interest_SpreadType2</t>
+  </si>
+  <si>
+    <t>Interest_SpreadValue1</t>
+  </si>
+  <si>
+    <t>Interest_SpreadAmt1</t>
+  </si>
+  <si>
+    <t>Interest_BaseRateCode1</t>
+  </si>
+  <si>
+    <t>Facility_PricingRuleOption1</t>
+  </si>
+  <si>
+    <t>Facility Ongoing Fee</t>
+  </si>
+  <si>
+    <t>FormulaCategory</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>1.75%</t>
+  </si>
+  <si>
+    <t>1.750000</t>
+  </si>
+  <si>
+    <t>Basis Points</t>
+  </si>
+  <si>
+    <t>Option</t>
+  </si>
+  <si>
+    <t>2.5</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>LIBOR</t>
+  </si>
+  <si>
+    <t>Fixed Rate Option</t>
+  </si>
+  <si>
+    <t>Primary_Lender</t>
+  </si>
+  <si>
+    <t>Primary_LenderLoc</t>
+  </si>
+  <si>
+    <t>Primary_RiskBook</t>
+  </si>
+  <si>
+    <t>Primary_PctOfDeal</t>
+  </si>
+  <si>
+    <t>BuySellPrice</t>
+  </si>
+  <si>
+    <t>SellAmount</t>
+  </si>
+  <si>
+    <t>Primary_Comment</t>
+  </si>
+  <si>
+    <t>Primary_Contact</t>
+  </si>
+  <si>
+    <t>Primary_SGAlias1</t>
+  </si>
+  <si>
+    <t>Primary_Portfolio</t>
+  </si>
+  <si>
+    <t>Primary_PortfolioBranch</t>
+  </si>
+  <si>
+    <t>Primary_PortfolioAllocation</t>
+  </si>
+  <si>
+    <t>PrimaryFacility1_Allocation</t>
+  </si>
+  <si>
+    <t>Primary_PortfolioExpiryDate</t>
+  </si>
+  <si>
+    <t>Primary_CircledDate</t>
+  </si>
+  <si>
+    <t>Expiry_Date</t>
+  </si>
+  <si>
+    <t>Structured Asset Finance</t>
+  </si>
+  <si>
+    <t>Origination</t>
+  </si>
+  <si>
+    <t>Add Comment</t>
+  </si>
+  <si>
+    <t>Hold for Investment - Europe</t>
+  </si>
+  <si>
+    <t>100,000.00</t>
+  </si>
+  <si>
+    <t>Facility_Spread</t>
+  </si>
+  <si>
+    <t>Facility_CurrentAvailToDraw</t>
+  </si>
+  <si>
+    <t>Facility_CurrentGlobalOutstandings</t>
+  </si>
+  <si>
+    <t>Outstanding_Type</t>
+  </si>
+  <si>
+    <t>Loan_FacilityName</t>
+  </si>
+  <si>
+    <t>Loan_Alias</t>
+  </si>
+  <si>
+    <t>Loan_PricingOption</t>
+  </si>
+  <si>
+    <t>Loan_Currency</t>
+  </si>
+  <si>
+    <t>Loan_RequestedAmount</t>
+  </si>
+  <si>
+    <t>HostBankSharePct</t>
+  </si>
+  <si>
+    <t>Loan_EffectiveDate</t>
+  </si>
+  <si>
+    <t>Loan_MaturityDate</t>
+  </si>
+  <si>
+    <t>Loan_RepricingFrequency</t>
+  </si>
+  <si>
+    <t>Loan_IntCycleFrequency</t>
+  </si>
+  <si>
+    <t>Loan_Accrue</t>
+  </si>
+  <si>
+    <t>Borrower_BaseRate</t>
+  </si>
+  <si>
+    <t>Repayment_ScheduleFrequency</t>
+  </si>
+  <si>
+    <t>Repayment_NumberOfCycles</t>
+  </si>
+  <si>
+    <t>Repayment_TriggerDate</t>
+  </si>
+  <si>
+    <t>Repayment_NonBusDayRule</t>
+  </si>
+  <si>
+    <t>WIP_TransactionType</t>
+  </si>
+  <si>
+    <t>WIP_AwaitingApprovalStatus</t>
+  </si>
+  <si>
+    <t>WIP_OutstandingType</t>
+  </si>
+  <si>
+    <t>WIP_AwaitingRateApprovalStatus</t>
+  </si>
+  <si>
+    <t>WIP_AwaitingReleaseCashflowsStatus</t>
+  </si>
+  <si>
+    <t>Borrower_Profile</t>
+  </si>
+  <si>
+    <t>Remittance_Status</t>
+  </si>
+  <si>
+    <t>Remittance_Description</t>
+  </si>
+  <si>
+    <t>HostBank_GLAccount</t>
+  </si>
+  <si>
+    <t>Borrower_GLAccount</t>
+  </si>
+  <si>
+    <t>Host_Bank</t>
+  </si>
+  <si>
+    <t>NoticeStatus</t>
+  </si>
+  <si>
+    <t>BranchCode</t>
+  </si>
+  <si>
+    <t>CEU_FAC_10062020130642XHO</t>
+  </si>
+  <si>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t>60000278</t>
+  </si>
+  <si>
+    <t>10000.00</t>
+  </si>
+  <si>
     <t>26-May-2025</t>
   </si>
   <si>
-    <t>Fixed Rate Loan</t>
-  </si>
-  <si>
-    <t>FLOAT</t>
-  </si>
-  <si>
-    <t>Working Capital</t>
-  </si>
-  <si>
-    <t>100.000000%</t>
-  </si>
-  <si>
-    <t>Facility B Partially Drawn</t>
-  </si>
-  <si>
-    <t>PARDRAW</t>
-  </si>
-  <si>
-    <t>Revolver</t>
-  </si>
-  <si>
-    <t>30,000,000.00</t>
-  </si>
-  <si>
-    <t>Loan</t>
-  </si>
-  <si>
-    <t>Facility Internal Undrawn</t>
-  </si>
-  <si>
-    <t>INTUND</t>
-  </si>
-  <si>
-    <t>20,000,000.00</t>
-  </si>
-  <si>
-    <t>OngoingFee_Category1</t>
-  </si>
-  <si>
-    <t>OngoingFee_Type1</t>
-  </si>
-  <si>
-    <t>OngoingFee_RateBasis1</t>
-  </si>
-  <si>
-    <t>OngoingFee_AfterItem</t>
-  </si>
-  <si>
-    <t>OngoingFee_AfterItemType</t>
-  </si>
-  <si>
-    <t>Facility_PercentWhole</t>
-  </si>
-  <si>
-    <t>Facility_Percent</t>
-  </si>
-  <si>
-    <t>OngoingFee_SpreadType1</t>
-  </si>
-  <si>
-    <t>OngoingFee_SpreadType2</t>
-  </si>
-  <si>
-    <t>Interest_AddItem</t>
-  </si>
-  <si>
-    <t>Interest_OptionName1</t>
-  </si>
-  <si>
-    <t>Interest_RateBasis</t>
-  </si>
-  <si>
-    <t>Interest_SpreadType1</t>
-  </si>
-  <si>
-    <t>Interest_SpreadType2</t>
-  </si>
-  <si>
-    <t>Interest_SpreadValue1</t>
-  </si>
-  <si>
-    <t>Interest_SpreadAmt1</t>
-  </si>
-  <si>
-    <t>Interest_BaseRateCode1</t>
-  </si>
-  <si>
-    <t>Facility_PricingRuleOption1</t>
-  </si>
-  <si>
-    <t>Facility Ongoing Fee</t>
-  </si>
-  <si>
-    <t>FormulaCategory</t>
-  </si>
-  <si>
-    <t>Normal</t>
-  </si>
-  <si>
-    <t>1.75%</t>
-  </si>
-  <si>
-    <t>1.750000</t>
-  </si>
-  <si>
-    <t>Basis Points</t>
-  </si>
-  <si>
-    <t>Option</t>
-  </si>
-  <si>
-    <t>2.5</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>LIBOR</t>
-  </si>
-  <si>
-    <t>Fixed Rate Option</t>
-  </si>
-  <si>
-    <t>Primary_Lender</t>
-  </si>
-  <si>
-    <t>Primary_LenderLoc</t>
-  </si>
-  <si>
-    <t>Primary_RiskBook</t>
-  </si>
-  <si>
-    <t>Primary_PctOfDeal</t>
-  </si>
-  <si>
-    <t>BuySellPrice</t>
-  </si>
-  <si>
-    <t>SellAmount</t>
-  </si>
-  <si>
-    <t>Primary_Comment</t>
-  </si>
-  <si>
-    <t>Primary_Contact</t>
-  </si>
-  <si>
-    <t>Primary_SGAlias1</t>
-  </si>
-  <si>
-    <t>Primary_Portfolio</t>
-  </si>
-  <si>
-    <t>Primary_PortfolioBranch</t>
-  </si>
-  <si>
-    <t>Primary_PortfolioAllocation</t>
-  </si>
-  <si>
-    <t>PrimaryFacility1_Allocation</t>
-  </si>
-  <si>
-    <t>Primary_PortfolioExpiryDate</t>
-  </si>
-  <si>
-    <t>Primary_CircledDate</t>
-  </si>
-  <si>
-    <t>Expiry_Date</t>
-  </si>
-  <si>
-    <t>Structured Asset Finance</t>
-  </si>
-  <si>
-    <t>Origination</t>
-  </si>
-  <si>
-    <t>Add Comment</t>
-  </si>
-  <si>
-    <t>Hold for Investment - Europe</t>
-  </si>
-  <si>
-    <t>100,000.00</t>
-  </si>
-  <si>
-    <t>Facility_Spread</t>
-  </si>
-  <si>
-    <t>Facility_CurrentAvailToDraw</t>
-  </si>
-  <si>
-    <t>Facility_CurrentGlobalOutstandings</t>
-  </si>
-  <si>
-    <t>Outstanding_Type</t>
-  </si>
-  <si>
-    <t>Loan_FacilityName</t>
-  </si>
-  <si>
-    <t>Loan_Alias</t>
-  </si>
-  <si>
-    <t>Loan_PricingOption</t>
-  </si>
-  <si>
-    <t>Loan_Currency</t>
-  </si>
-  <si>
-    <t>Loan_RequestedAmount</t>
-  </si>
-  <si>
-    <t>HostBankSharePct</t>
-  </si>
-  <si>
-    <t>Loan_EffectiveDate</t>
-  </si>
-  <si>
-    <t>Loan_MaturityDate</t>
-  </si>
-  <si>
-    <t>Loan_RepricingFrequency</t>
-  </si>
-  <si>
-    <t>Loan_IntCycleFrequency</t>
-  </si>
-  <si>
-    <t>Loan_Accrue</t>
-  </si>
-  <si>
-    <t>Borrower_BaseRate</t>
-  </si>
-  <si>
-    <t>Repayment_ScheduleFrequency</t>
-  </si>
-  <si>
-    <t>Repayment_NumberOfCycles</t>
-  </si>
-  <si>
-    <t>Repayment_TriggerDate</t>
-  </si>
-  <si>
-    <t>Repayment_NonBusDayRule</t>
-  </si>
-  <si>
-    <t>WIP_TransactionType</t>
-  </si>
-  <si>
-    <t>WIP_AwaitingApprovalStatus</t>
-  </si>
-  <si>
-    <t>WIP_OutstandingType</t>
-  </si>
-  <si>
-    <t>WIP_AwaitingRateApprovalStatus</t>
-  </si>
-  <si>
-    <t>WIP_AwaitingReleaseCashflowsStatus</t>
-  </si>
-  <si>
-    <t>Borrower_Profile</t>
-  </si>
-  <si>
-    <t>Remittance_Status</t>
-  </si>
-  <si>
-    <t>Remittance_Description</t>
-  </si>
-  <si>
-    <t>HostBank_GLAccount</t>
-  </si>
-  <si>
-    <t>Borrower_GLAccount</t>
-  </si>
-  <si>
-    <t>Host_Bank</t>
-  </si>
-  <si>
-    <t>NoticeStatus</t>
-  </si>
-  <si>
-    <t>BranchCode</t>
-  </si>
-  <si>
-    <t>CEU_FAC_10062020130642XHO</t>
-  </si>
-  <si>
-    <t>0.00</t>
-  </si>
-  <si>
-    <t>60000278</t>
-  </si>
-  <si>
-    <t>10000.00</t>
-  </si>
-  <si>
     <t>Monthly</t>
   </si>
   <si>
@@ -2134,9 +2198,6 @@
     <t>Outstandings</t>
   </si>
   <si>
-    <t>Awaiting Approval</t>
-  </si>
-  <si>
     <t>Loan Initial Drawdown</t>
   </si>
   <si>
@@ -2266,9 +2327,6 @@
     <t>TRN02</t>
   </si>
   <si>
-    <t>22-May-2020</t>
-  </si>
-  <si>
     <t>This is to update or Modify the Onging Fee and Interest Pricing.</t>
   </si>
   <si>
@@ -2492,9 +2550,6 @@
   </si>
   <si>
     <t>90.41</t>
-  </si>
-  <si>
-    <t>Payments</t>
   </si>
   <si>
     <t>Interest Payment</t>
@@ -2598,7 +2653,7 @@
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="m/d/yy"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2704,8 +2759,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2757,6 +2819,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="51"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2837,7 +2905,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2967,6 +3035,13 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3290,8 +3365,8 @@
   <dimension ref="A1:CW2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AU1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AW2" sqref="AW1:AW2"/>
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3527,9 +3602,7 @@
       <c r="AV1" s="75" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="75" t="s">
-        <v>295</v>
-      </c>
+      <c r="AW1" s="75"/>
       <c r="AX1" s="75"/>
       <c r="AY1" s="75"/>
       <c r="AZ1" s="75"/>
@@ -3728,9 +3801,6 @@
       <c r="AV2" s="86" t="s">
         <v>86</v>
       </c>
-      <c r="AW2" s="86" t="s">
-        <v>392</v>
-      </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
@@ -3740,15 +3810,13 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AQ2"/>
+  <dimension ref="A1:AP2"/>
   <sheetViews>
-    <sheetView topLeftCell="AI1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AQ1" sqref="AQ1:AQ2"/>
-    </sheetView>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3794,7 +3862,7 @@
     <col min="42" max="42" width="23.42578125" style="86" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -3808,124 +3876,121 @@
         <v>421</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>706</v>
+        <v>726</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>707</v>
+        <v>727</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>708</v>
+        <v>728</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>709</v>
+        <v>729</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>710</v>
+        <v>730</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>711</v>
+        <v>731</v>
       </c>
       <c r="K1" s="16" t="s">
-        <v>712</v>
+        <v>732</v>
       </c>
       <c r="L1" s="16" t="s">
-        <v>713</v>
+        <v>733</v>
       </c>
       <c r="M1" s="16" t="s">
-        <v>714</v>
+        <v>734</v>
       </c>
       <c r="N1" s="16" t="s">
-        <v>715</v>
+        <v>735</v>
       </c>
       <c r="O1" s="16" t="s">
-        <v>716</v>
+        <v>736</v>
       </c>
       <c r="P1" s="16" t="s">
-        <v>717</v>
+        <v>737</v>
       </c>
       <c r="Q1" s="16" t="s">
-        <v>718</v>
+        <v>738</v>
       </c>
       <c r="R1" s="16" t="s">
-        <v>719</v>
+        <v>739</v>
       </c>
       <c r="S1" s="16" t="s">
-        <v>720</v>
+        <v>740</v>
       </c>
       <c r="T1" s="16" t="s">
-        <v>721</v>
+        <v>741</v>
       </c>
       <c r="U1" s="16" t="s">
-        <v>722</v>
+        <v>742</v>
       </c>
       <c r="V1" s="16" t="s">
-        <v>723</v>
+        <v>743</v>
       </c>
       <c r="W1" s="16" t="s">
-        <v>724</v>
+        <v>744</v>
       </c>
       <c r="X1" s="16" t="s">
-        <v>725</v>
+        <v>745</v>
       </c>
       <c r="Y1" s="16" t="s">
-        <v>726</v>
+        <v>746</v>
       </c>
       <c r="Z1" s="16" t="s">
-        <v>727</v>
+        <v>747</v>
       </c>
       <c r="AA1" s="16" t="s">
-        <v>728</v>
+        <v>748</v>
       </c>
       <c r="AB1" s="16" t="s">
-        <v>729</v>
+        <v>749</v>
       </c>
       <c r="AC1" s="16" t="s">
-        <v>730</v>
+        <v>750</v>
       </c>
       <c r="AD1" s="16" t="s">
-        <v>731</v>
+        <v>751</v>
       </c>
       <c r="AE1" s="16" t="s">
-        <v>732</v>
+        <v>752</v>
       </c>
       <c r="AF1" s="16" t="s">
-        <v>733</v>
+        <v>753</v>
       </c>
       <c r="AG1" s="16" t="s">
-        <v>734</v>
+        <v>754</v>
       </c>
       <c r="AH1" s="16" t="s">
-        <v>735</v>
+        <v>755</v>
       </c>
       <c r="AI1" s="2" t="s">
-        <v>611</v>
+        <v>631</v>
       </c>
       <c r="AJ1" s="2" t="s">
-        <v>612</v>
+        <v>632</v>
       </c>
       <c r="AK1" s="2" t="s">
-        <v>613</v>
+        <v>633</v>
       </c>
       <c r="AL1" s="2" t="s">
-        <v>614</v>
+        <v>634</v>
       </c>
       <c r="AM1" s="2" t="s">
-        <v>615</v>
+        <v>635</v>
       </c>
       <c r="AN1" s="2" t="s">
-        <v>616</v>
+        <v>636</v>
       </c>
       <c r="AO1" s="2" t="s">
-        <v>617</v>
+        <v>637</v>
       </c>
       <c r="AP1" s="2" t="s">
-        <v>618</v>
-      </c>
-      <c r="AQ1" s="75" t="s">
-        <v>295</v>
+        <v>638</v>
       </c>
     </row>
-    <row r="2" spans="1:43" s="86" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42" s="86" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="86" t="s">
         <v>48</v>
       </c>
@@ -3933,125 +3998,122 @@
         <v>297</v>
       </c>
       <c r="C2" s="86" t="s">
-        <v>736</v>
+        <v>756</v>
       </c>
       <c r="D2" s="86" t="s">
-        <v>685</v>
+        <v>705</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>737</v>
+        <v>757</v>
       </c>
       <c r="F2" s="18"/>
       <c r="G2" s="18" t="s">
-        <v>738</v>
+        <v>758</v>
       </c>
       <c r="H2" s="86" t="s">
-        <v>739</v>
+        <v>532</v>
       </c>
       <c r="I2" s="19" t="s">
-        <v>740</v>
+        <v>759</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>620</v>
+        <v>640</v>
       </c>
       <c r="K2" s="18" t="s">
         <v>541</v>
       </c>
       <c r="L2" s="18" t="s">
-        <v>621</v>
+        <v>641</v>
       </c>
       <c r="M2" s="18" t="s">
-        <v>622</v>
+        <v>642</v>
       </c>
       <c r="N2" s="20" t="s">
-        <v>628</v>
+        <v>648</v>
       </c>
       <c r="O2" s="20" t="s">
-        <v>741</v>
+        <v>760</v>
       </c>
       <c r="P2" s="21" t="s">
-        <v>742</v>
+        <v>761</v>
       </c>
       <c r="Q2" s="18" t="s">
-        <v>743</v>
+        <v>762</v>
       </c>
       <c r="R2" s="18" t="s">
-        <v>744</v>
+        <v>763</v>
       </c>
       <c r="S2" s="86" t="s">
-        <v>742</v>
+        <v>761</v>
       </c>
       <c r="T2" s="18" t="s">
-        <v>744</v>
+        <v>763</v>
       </c>
       <c r="U2" s="86" t="s">
-        <v>742</v>
+        <v>761</v>
       </c>
       <c r="V2" s="18" t="s">
-        <v>745</v>
+        <v>764</v>
       </c>
       <c r="W2" s="18" t="s">
-        <v>746</v>
+        <v>765</v>
       </c>
       <c r="X2" s="18" t="s">
-        <v>747</v>
+        <v>766</v>
       </c>
       <c r="Y2" s="18" t="s">
-        <v>748</v>
+        <v>767</v>
       </c>
       <c r="Z2" s="18" t="s">
-        <v>749</v>
+        <v>768</v>
       </c>
       <c r="AA2" s="18" t="s">
-        <v>750</v>
+        <v>769</v>
       </c>
       <c r="AB2" s="18" t="s">
-        <v>751</v>
+        <v>770</v>
       </c>
       <c r="AC2" s="18" t="s">
-        <v>752</v>
+        <v>771</v>
       </c>
       <c r="AD2" s="18" t="s">
-        <v>753</v>
+        <v>772</v>
       </c>
       <c r="AE2" s="18" t="s">
-        <v>754</v>
+        <v>773</v>
       </c>
       <c r="AF2" s="86" t="s">
-        <v>755</v>
+        <v>774</v>
       </c>
       <c r="AG2" s="18" t="s">
-        <v>756</v>
+        <v>775</v>
       </c>
       <c r="AH2" s="18" t="s">
-        <v>620</v>
+        <v>640</v>
       </c>
       <c r="AI2" s="86" t="s">
-        <v>626</v>
+        <v>646</v>
       </c>
       <c r="AJ2" s="22" t="s">
-        <v>630</v>
+        <v>650</v>
       </c>
       <c r="AK2" s="86" t="s">
-        <v>741</v>
+        <v>760</v>
       </c>
       <c r="AL2" s="5" t="s">
-        <v>555</v>
+        <v>575</v>
       </c>
       <c r="AM2" s="4" t="s">
-        <v>625</v>
+        <v>645</v>
       </c>
       <c r="AN2" s="86" t="s">
-        <v>757</v>
+        <v>776</v>
       </c>
       <c r="AO2" s="86" t="s">
-        <v>757</v>
+        <v>776</v>
       </c>
       <c r="AP2" s="86" t="s">
-        <v>758</v>
-      </c>
-      <c r="AQ2" s="86" t="s">
-        <v>392</v>
+        <v>777</v>
       </c>
     </row>
   </sheetData>
@@ -4062,15 +4124,13 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G2"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4082,7 +4142,7 @@
     <col min="6" max="6" width="15.28515625" style="86" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -4093,39 +4153,33 @@
         <v>419</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>759</v>
+        <v>778</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>760</v>
+        <v>779</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>761</v>
-      </c>
-      <c r="G1" s="75" t="s">
-        <v>295</v>
+        <v>780</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="86" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" s="86" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="86" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="86" t="s">
-        <v>762</v>
+        <v>781</v>
       </c>
       <c r="C2" s="86" t="s">
-        <v>763</v>
+        <v>782</v>
       </c>
       <c r="D2" s="86" t="s">
-        <v>739</v>
+        <v>532</v>
       </c>
       <c r="E2" s="86" t="s">
-        <v>764</v>
+        <v>783</v>
       </c>
       <c r="F2" s="86">
         <v>2</v>
-      </c>
-      <c r="G2" s="86" t="s">
-        <v>392</v>
       </c>
     </row>
   </sheetData>
@@ -4136,15 +4190,15 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:CW2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="X1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AD1" sqref="AD1:AD2"/>
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4263,82 +4317,79 @@
         <v>421</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>765</v>
+        <v>784</v>
       </c>
       <c r="F1" s="34" t="s">
         <v>426</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>766</v>
+        <v>785</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>767</v>
+        <v>786</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>657</v>
+        <v>677</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>768</v>
+        <v>787</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>166</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>678</v>
+        <v>698</v>
       </c>
       <c r="M1" s="13" t="s">
-        <v>769</v>
+        <v>788</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>659</v>
+        <v>679</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>176</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>677</v>
+        <v>697</v>
       </c>
       <c r="Q1" s="12" t="s">
-        <v>770</v>
+        <v>789</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>771</v>
+        <v>790</v>
       </c>
       <c r="S1" s="13" t="s">
-        <v>662</v>
+        <v>682</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>772</v>
+        <v>791</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>681</v>
+        <v>701</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>680</v>
+        <v>700</v>
       </c>
       <c r="W1" s="13" t="s">
-        <v>773</v>
+        <v>792</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>774</v>
+        <v>793</v>
       </c>
       <c r="Y1" s="2" t="s">
-        <v>775</v>
+        <v>794</v>
       </c>
       <c r="Z1" s="2" t="s">
-        <v>560</v>
+        <v>580</v>
       </c>
       <c r="AA1" s="2" t="s">
         <v>227</v>
       </c>
       <c r="AB1" s="13" t="s">
-        <v>661</v>
+        <v>681</v>
       </c>
       <c r="AC1" s="13" t="s">
-        <v>682</v>
-      </c>
-      <c r="AD1" s="75" t="s">
-        <v>295</v>
+        <v>702</v>
       </c>
       <c r="AX1" s="36"/>
       <c r="AY1" s="36"/>
@@ -4401,25 +4452,25 @@
         <v>297</v>
       </c>
       <c r="C2" s="86" t="s">
-        <v>736</v>
+        <v>756</v>
       </c>
       <c r="D2" s="86" t="s">
-        <v>685</v>
+        <v>705</v>
       </c>
       <c r="E2" s="86" t="s">
-        <v>776</v>
+        <v>795</v>
       </c>
       <c r="F2" s="86" t="s">
         <v>306</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>598</v>
+        <v>618</v>
       </c>
       <c r="H2" s="86" t="s">
-        <v>777</v>
+        <v>796</v>
       </c>
       <c r="I2" s="86" t="s">
-        <v>778</v>
+        <v>797</v>
       </c>
       <c r="J2" s="86" t="s">
         <v>308</v>
@@ -4428,7 +4479,7 @@
         <v>300</v>
       </c>
       <c r="L2" s="86" t="s">
-        <v>700</v>
+        <v>720</v>
       </c>
       <c r="M2" s="86" t="s">
         <v>307</v>
@@ -4437,49 +4488,46 @@
         <v>361</v>
       </c>
       <c r="O2" s="86" t="s">
-        <v>779</v>
+        <v>798</v>
       </c>
       <c r="P2" s="86" t="s">
         <v>322</v>
       </c>
       <c r="Q2" s="86" t="s">
-        <v>780</v>
+        <v>799</v>
       </c>
       <c r="R2" s="86" t="s">
         <v>48</v>
       </c>
       <c r="S2" s="86" t="s">
-        <v>739</v>
+        <v>532</v>
       </c>
       <c r="U2" s="86" t="s">
-        <v>702</v>
+        <v>722</v>
       </c>
       <c r="V2" s="86" t="s">
-        <v>701</v>
+        <v>721</v>
       </c>
       <c r="W2" s="86" t="s">
-        <v>739</v>
+        <v>532</v>
       </c>
       <c r="X2" s="86" t="s">
-        <v>781</v>
+        <v>800</v>
       </c>
       <c r="Y2" s="86" t="s">
-        <v>651</v>
+        <v>671</v>
       </c>
       <c r="Z2" s="86" t="s">
-        <v>587</v>
+        <v>607</v>
       </c>
       <c r="AA2" s="31" t="s">
-        <v>782</v>
+        <v>801</v>
       </c>
       <c r="AB2" s="32">
         <v>100</v>
       </c>
       <c r="AC2" s="86" t="s">
-        <v>783</v>
-      </c>
-      <c r="AD2" s="86" t="s">
-        <v>392</v>
+        <v>802</v>
       </c>
     </row>
   </sheetData>
@@ -4490,15 +4538,13 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AU4"/>
+  <dimension ref="A1:AT4"/>
   <sheetViews>
-    <sheetView topLeftCell="AP1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AU1" sqref="AU1:AU2"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4548,7 +4594,7 @@
     <col min="46" max="46" width="40.85546875" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" s="1" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:46" s="1" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
@@ -4559,31 +4605,31 @@
         <v>419</v>
       </c>
       <c r="D1" s="37" t="s">
-        <v>560</v>
+        <v>580</v>
       </c>
       <c r="E1" s="39" t="s">
         <v>421</v>
       </c>
       <c r="F1" s="26" t="s">
-        <v>784</v>
+        <v>803</v>
       </c>
       <c r="G1" s="26" t="s">
-        <v>785</v>
+        <v>804</v>
       </c>
       <c r="H1" s="39" t="s">
-        <v>786</v>
+        <v>805</v>
       </c>
       <c r="I1" s="39" t="s">
-        <v>657</v>
+        <v>677</v>
       </c>
       <c r="J1" s="37" t="s">
-        <v>658</v>
+        <v>678</v>
       </c>
       <c r="K1" s="26" t="s">
-        <v>787</v>
+        <v>806</v>
       </c>
       <c r="L1" s="26" t="s">
-        <v>788</v>
+        <v>807</v>
       </c>
       <c r="M1" s="40" t="s">
         <v>174</v>
@@ -4592,64 +4638,64 @@
         <v>426</v>
       </c>
       <c r="O1" s="37" t="s">
-        <v>789</v>
+        <v>808</v>
       </c>
       <c r="P1" s="41" t="s">
-        <v>790</v>
+        <v>809</v>
       </c>
       <c r="Q1" s="42" t="s">
-        <v>791</v>
+        <v>810</v>
       </c>
       <c r="R1" s="37" t="s">
-        <v>792</v>
+        <v>811</v>
       </c>
       <c r="S1" s="39" t="s">
-        <v>793</v>
+        <v>812</v>
       </c>
       <c r="T1" s="39" t="s">
-        <v>794</v>
+        <v>813</v>
       </c>
       <c r="U1" s="39" t="s">
-        <v>795</v>
+        <v>814</v>
       </c>
       <c r="V1" s="39" t="s">
-        <v>796</v>
+        <v>815</v>
       </c>
       <c r="W1" s="26" t="s">
-        <v>797</v>
+        <v>816</v>
       </c>
       <c r="X1" s="25" t="s">
-        <v>798</v>
+        <v>817</v>
       </c>
       <c r="Y1" s="25" t="s">
-        <v>799</v>
+        <v>818</v>
       </c>
       <c r="Z1" s="25" t="s">
-        <v>800</v>
+        <v>819</v>
       </c>
       <c r="AA1" s="39" t="s">
         <v>227</v>
       </c>
       <c r="AB1" s="39" t="s">
-        <v>801</v>
+        <v>820</v>
       </c>
       <c r="AC1" s="26" t="s">
-        <v>655</v>
+        <v>675</v>
       </c>
       <c r="AD1" s="26" t="s">
-        <v>672</v>
+        <v>692</v>
       </c>
       <c r="AE1" s="26" t="s">
-        <v>673</v>
+        <v>693</v>
       </c>
       <c r="AF1" s="26" t="s">
-        <v>802</v>
+        <v>821</v>
       </c>
       <c r="AG1" s="26" t="s">
-        <v>676</v>
+        <v>696</v>
       </c>
       <c r="AH1" s="26" t="s">
-        <v>677</v>
+        <v>697</v>
       </c>
       <c r="AI1" s="25" t="s">
         <v>176</v>
@@ -4658,40 +4704,37 @@
         <v>166</v>
       </c>
       <c r="AK1" s="26" t="s">
-        <v>678</v>
+        <v>698</v>
       </c>
       <c r="AL1" s="26" t="s">
-        <v>659</v>
+        <v>679</v>
       </c>
       <c r="AM1" s="25" t="s">
         <v>166</v>
       </c>
       <c r="AN1" s="25" t="s">
-        <v>803</v>
+        <v>822</v>
       </c>
       <c r="AO1" s="43" t="s">
-        <v>768</v>
+        <v>787</v>
       </c>
       <c r="AP1" s="25" t="s">
-        <v>804</v>
+        <v>823</v>
       </c>
       <c r="AQ1" s="25" t="s">
-        <v>680</v>
+        <v>700</v>
       </c>
       <c r="AR1" s="25" t="s">
+        <v>701</v>
+      </c>
+      <c r="AS1" s="25" t="s">
         <v>681</v>
       </c>
-      <c r="AS1" s="25" t="s">
-        <v>661</v>
-      </c>
       <c r="AT1" s="25" t="s">
-        <v>682</v>
-      </c>
-      <c r="AU1" s="75" t="s">
-        <v>295</v>
+        <v>702</v>
       </c>
     </row>
-    <row r="2" spans="1:47" s="86" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="86" t="s">
         <v>48</v>
       </c>
@@ -4699,31 +4742,31 @@
         <v>297</v>
       </c>
       <c r="C2" s="86" t="s">
-        <v>736</v>
+        <v>756</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>587</v>
+        <v>607</v>
       </c>
       <c r="E2" s="86" t="s">
-        <v>685</v>
+        <v>705</v>
       </c>
       <c r="F2" s="86" t="s">
-        <v>805</v>
+        <v>824</v>
       </c>
       <c r="G2" s="86" t="s">
-        <v>806</v>
+        <v>825</v>
       </c>
       <c r="H2" s="86" t="s">
         <v>306</v>
       </c>
       <c r="I2" s="86" t="s">
-        <v>687</v>
+        <v>707</v>
       </c>
       <c r="K2" s="86" t="s">
-        <v>807</v>
+        <v>826</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>808</v>
+        <v>827</v>
       </c>
       <c r="M2" s="86" t="s">
         <v>306</v>
@@ -4732,7 +4775,7 @@
         <v>306</v>
       </c>
       <c r="O2" s="86" t="s">
-        <v>809</v>
+        <v>828</v>
       </c>
       <c r="P2" s="86" t="s">
         <v>48</v>
@@ -4741,22 +4784,22 @@
         <v>48</v>
       </c>
       <c r="R2" s="86" t="s">
-        <v>810</v>
+        <v>829</v>
       </c>
       <c r="S2" s="86" t="s">
-        <v>811</v>
+        <v>830</v>
       </c>
       <c r="T2" s="86" t="s">
-        <v>812</v>
+        <v>831</v>
       </c>
       <c r="U2" s="86" t="s">
-        <v>813</v>
+        <v>832</v>
       </c>
       <c r="V2" s="86" t="s">
-        <v>739</v>
+        <v>532</v>
       </c>
       <c r="W2" s="15" t="s">
-        <v>704</v>
+        <v>724</v>
       </c>
       <c r="X2" s="31" t="s">
         <v>347</v>
@@ -4767,67 +4810,64 @@
         <v>347</v>
       </c>
       <c r="AB2" s="86" t="s">
-        <v>814</v>
+        <v>833</v>
       </c>
       <c r="AC2" s="86" t="s">
-        <v>598</v>
+        <v>618</v>
       </c>
       <c r="AD2" s="86" t="s">
-        <v>815</v>
+        <v>566</v>
       </c>
       <c r="AE2" s="86" t="s">
-        <v>695</v>
+        <v>567</v>
       </c>
       <c r="AF2" s="86" t="s">
-        <v>816</v>
+        <v>834</v>
       </c>
       <c r="AG2" s="15" t="s">
-        <v>698</v>
+        <v>718</v>
       </c>
       <c r="AH2" s="15" t="s">
         <v>322</v>
       </c>
       <c r="AI2" s="86" t="s">
-        <v>779</v>
+        <v>798</v>
       </c>
       <c r="AJ2" s="86" t="s">
         <v>300</v>
       </c>
       <c r="AK2" s="86" t="s">
-        <v>700</v>
+        <v>720</v>
       </c>
       <c r="AL2" s="86" t="s">
         <v>361</v>
       </c>
       <c r="AM2" s="86" t="s">
-        <v>817</v>
+        <v>835</v>
       </c>
       <c r="AN2" s="86" t="s">
-        <v>818</v>
+        <v>836</v>
       </c>
       <c r="AO2" s="86" t="s">
         <v>308</v>
       </c>
       <c r="AP2" s="86" t="s">
-        <v>818</v>
+        <v>836</v>
       </c>
       <c r="AQ2" s="32" t="s">
-        <v>819</v>
+        <v>837</v>
       </c>
       <c r="AR2" s="32" t="s">
-        <v>702</v>
+        <v>722</v>
       </c>
       <c r="AS2" s="32">
         <v>100</v>
       </c>
       <c r="AT2" s="86" t="s">
-        <v>783</v>
-      </c>
-      <c r="AU2" s="86" t="s">
-        <v>392</v>
+        <v>802</v>
       </c>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
       <c r="N4" s="44"/>
     </row>
   </sheetData>
@@ -4838,15 +4878,15 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AM5"/>
+  <dimension ref="A1:AL5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AH1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AM1" sqref="AM1:AM2"/>
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4890,7 +4930,7 @@
     <col min="38" max="38" width="14.7109375" style="86" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -4898,49 +4938,49 @@
         <v>1</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>820</v>
+        <v>838</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>785</v>
+        <v>804</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>821</v>
+        <v>839</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>822</v>
+        <v>840</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>823</v>
+        <v>841</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>824</v>
+        <v>842</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>768</v>
+        <v>787</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>657</v>
+        <v>677</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>825</v>
+        <v>843</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>678</v>
+        <v>698</v>
       </c>
       <c r="M1" s="13" t="s">
         <v>426</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>682</v>
+        <v>702</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>659</v>
+        <v>679</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>176</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>677</v>
+        <v>697</v>
       </c>
       <c r="R1" s="34" t="s">
         <v>421</v>
@@ -4949,67 +4989,64 @@
         <v>419</v>
       </c>
       <c r="T1" s="34" t="s">
-        <v>770</v>
+        <v>789</v>
       </c>
       <c r="U1" s="12" t="s">
-        <v>826</v>
+        <v>844</v>
       </c>
       <c r="V1" s="34" t="s">
-        <v>827</v>
+        <v>845</v>
       </c>
       <c r="W1" s="34" t="s">
-        <v>828</v>
+        <v>846</v>
       </c>
       <c r="X1" s="34" t="s">
-        <v>829</v>
+        <v>847</v>
       </c>
       <c r="Y1" s="12" t="s">
-        <v>771</v>
+        <v>790</v>
       </c>
       <c r="Z1" s="2" t="s">
-        <v>830</v>
+        <v>848</v>
       </c>
       <c r="AA1" s="2" t="s">
-        <v>831</v>
+        <v>849</v>
       </c>
       <c r="AB1" s="2" t="s">
-        <v>832</v>
+        <v>850</v>
       </c>
       <c r="AC1" s="2" t="s">
-        <v>661</v>
+        <v>681</v>
       </c>
       <c r="AD1" s="2" t="s">
-        <v>716</v>
+        <v>736</v>
       </c>
       <c r="AE1" s="2" t="s">
-        <v>833</v>
+        <v>851</v>
       </c>
       <c r="AF1" s="2" t="s">
-        <v>791</v>
+        <v>810</v>
       </c>
       <c r="AG1" s="2" t="s">
-        <v>834</v>
+        <v>852</v>
       </c>
       <c r="AH1" s="2" t="s">
         <v>227</v>
       </c>
       <c r="AI1" s="2" t="s">
-        <v>835</v>
+        <v>853</v>
       </c>
       <c r="AJ1" s="13" t="s">
-        <v>787</v>
+        <v>806</v>
       </c>
       <c r="AK1" s="2" t="s">
-        <v>836</v>
+        <v>854</v>
       </c>
       <c r="AL1" s="2" t="s">
-        <v>683</v>
-      </c>
-      <c r="AM1" s="75" t="s">
-        <v>295</v>
+        <v>703</v>
       </c>
     </row>
-    <row r="2" spans="1:39" s="86" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:38" s="86" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="86" t="s">
         <v>48</v>
       </c>
@@ -5017,16 +5054,16 @@
         <v>297</v>
       </c>
       <c r="C2" s="86" t="s">
-        <v>837</v>
+        <v>855</v>
       </c>
       <c r="D2" s="86" t="s">
-        <v>838</v>
+        <v>856</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>325</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>839</v>
+        <v>857</v>
       </c>
       <c r="G2" s="86" t="s">
         <v>515</v>
@@ -5035,37 +5072,37 @@
         <v>300</v>
       </c>
       <c r="J2" s="86" t="s">
-        <v>840</v>
+        <v>858</v>
       </c>
       <c r="K2" s="86" t="s">
         <v>308</v>
       </c>
       <c r="L2" s="86" t="s">
-        <v>700</v>
+        <v>720</v>
       </c>
       <c r="M2" s="86" t="s">
         <v>306</v>
       </c>
       <c r="N2" s="86" t="s">
-        <v>783</v>
+        <v>802</v>
       </c>
       <c r="O2" s="86" t="s">
         <v>361</v>
       </c>
       <c r="P2" s="86" t="s">
-        <v>779</v>
+        <v>798</v>
       </c>
       <c r="Q2" s="86" t="s">
         <v>322</v>
       </c>
       <c r="R2" s="86" t="s">
-        <v>685</v>
+        <v>705</v>
       </c>
       <c r="S2" s="86" t="s">
         <v>515</v>
       </c>
       <c r="T2" s="86" t="s">
-        <v>841</v>
+        <v>859</v>
       </c>
       <c r="U2" s="86" t="s">
         <v>541</v>
@@ -5080,49 +5117,46 @@
         <v>532</v>
       </c>
       <c r="Y2" s="86" t="s">
-        <v>842</v>
+        <v>860</v>
       </c>
       <c r="Z2" s="86">
         <v>69.040000000000006</v>
       </c>
       <c r="AB2" s="45" t="s">
-        <v>843</v>
+        <v>861</v>
       </c>
       <c r="AC2" s="45" t="s">
         <v>368</v>
       </c>
       <c r="AD2" s="86" t="s">
-        <v>741</v>
+        <v>760</v>
       </c>
       <c r="AE2" s="86" t="s">
-        <v>741</v>
+        <v>760</v>
       </c>
       <c r="AF2" s="86" t="s">
         <v>48</v>
       </c>
       <c r="AG2" s="86" t="s">
-        <v>844</v>
+        <v>862</v>
       </c>
       <c r="AH2" s="31" t="s">
-        <v>782</v>
+        <v>801</v>
       </c>
       <c r="AI2" s="86" t="s">
         <v>38</v>
       </c>
       <c r="AJ2" s="86" t="s">
-        <v>845</v>
+        <v>863</v>
       </c>
       <c r="AK2" s="86" t="s">
-        <v>846</v>
+        <v>864</v>
       </c>
       <c r="AL2" s="86" t="s">
-        <v>704</v>
-      </c>
-      <c r="AM2" s="86" t="s">
-        <v>392</v>
+        <v>724</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.2">
       <c r="C3" s="11"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -5130,14 +5164,14 @@
       <c r="AC3" s="45"/>
       <c r="AH3" s="31"/>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.2">
       <c r="X4" s="27"/>
       <c r="Z4" s="11"/>
       <c r="AA4" s="11"/>
       <c r="AB4" s="11"/>
       <c r="AC4" s="11"/>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.2">
       <c r="X5" s="27"/>
       <c r="Z5" s="11"/>
       <c r="AA5" s="11"/>
@@ -5152,14 +5186,14 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5172,7 +5206,7 @@
     <col min="6" max="6" width="15.28515625" style="86" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -5183,45 +5217,167 @@
         <v>419</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>759</v>
+        <v>778</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>760</v>
+        <v>779</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>761</v>
-      </c>
-      <c r="G1" s="75" t="s">
-        <v>295</v>
+        <v>780</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="86" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" s="86" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="86" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="86" t="s">
-        <v>762</v>
+        <v>781</v>
       </c>
       <c r="C2" s="86" t="s">
-        <v>736</v>
+        <v>756</v>
       </c>
       <c r="D2" s="86" t="s">
-        <v>739</v>
+        <v>532</v>
       </c>
       <c r="E2" s="86" t="s">
-        <v>764</v>
+        <v>783</v>
       </c>
       <c r="F2" s="86">
         <v>2</v>
-      </c>
-      <c r="G2" s="86" t="s">
-        <v>392</v>
       </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
   <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.85546875" style="88" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28" style="88" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44" style="88" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.28515625" style="88" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="21.7109375" style="88" customWidth="1"/>
+    <col min="7" max="7" width="36.7109375" style="88" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.7109375" style="88" customWidth="1"/>
+    <col min="9" max="9" width="35.7109375" style="88" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.28515625" style="88" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" style="88" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" style="88" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.5703125" style="88" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.140625" style="88" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="32.7109375" style="88" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.7109375" style="88" customWidth="1"/>
+    <col min="17" max="16384" width="8.7109375" style="88"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="89" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="87" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="87" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="92" t="s">
+        <v>419</v>
+      </c>
+      <c r="D1" s="92" t="s">
+        <v>421</v>
+      </c>
+      <c r="E1" s="87" t="s">
+        <v>555</v>
+      </c>
+      <c r="F1" s="87" t="s">
+        <v>556</v>
+      </c>
+      <c r="G1" s="87" t="s">
+        <v>557</v>
+      </c>
+      <c r="H1" s="87" t="s">
+        <v>558</v>
+      </c>
+      <c r="I1" s="87" t="s">
+        <v>559</v>
+      </c>
+      <c r="J1" s="93" t="s">
+        <v>560</v>
+      </c>
+      <c r="K1" s="89" t="s">
+        <v>561</v>
+      </c>
+      <c r="L1" s="89" t="s">
+        <v>562</v>
+      </c>
+      <c r="M1" s="89" t="s">
+        <v>563</v>
+      </c>
+      <c r="N1" s="89" t="s">
+        <v>564</v>
+      </c>
+      <c r="O1" s="89" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="86" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="86" t="s">
+        <v>512</v>
+      </c>
+      <c r="C2" s="86" t="s">
+        <v>515</v>
+      </c>
+      <c r="D2" s="86" t="s">
+        <v>517</v>
+      </c>
+      <c r="E2" s="86" t="s">
+        <v>306</v>
+      </c>
+      <c r="F2" s="86" t="s">
+        <v>566</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>567</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>568</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>569</v>
+      </c>
+      <c r="J2" s="86" t="s">
+        <v>517</v>
+      </c>
+      <c r="K2" s="90">
+        <v>4000</v>
+      </c>
+      <c r="L2" s="88" t="s">
+        <v>570</v>
+      </c>
+      <c r="M2" s="91" t="s">
+        <v>571</v>
+      </c>
+      <c r="N2" s="88" t="s">
+        <v>572</v>
+      </c>
+      <c r="O2" s="88" t="s">
+        <v>573</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
@@ -5233,13 +5389,13 @@
   <dimension ref="A1:AS8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AO2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AR1" sqref="AR1:AR2"/>
+      <selection pane="bottomRight" activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" style="64" customWidth="1"/>
     <col min="2" max="2" width="32.7109375" style="64" customWidth="1"/>
@@ -5278,11 +5434,11 @@
     <col min="42" max="42" width="8.7109375" style="64" customWidth="1"/>
     <col min="43" max="43" width="11.28515625" style="64" customWidth="1"/>
     <col min="44" max="45" width="8.7109375" style="64" customWidth="1"/>
-    <col min="46" max="62" width="9.140625" style="68" customWidth="1"/>
-    <col min="63" max="16384" width="9.140625" style="68"/>
+    <col min="46" max="64" width="9.140625" style="68" customWidth="1"/>
+    <col min="65" max="16384" width="9.140625" style="68"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" s="61" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" s="61" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
@@ -5412,11 +5568,8 @@
       <c r="AQ1" s="60" t="s">
         <v>128</v>
       </c>
-      <c r="AR1" s="75" t="s">
-        <v>295</v>
-      </c>
     </row>
-    <row r="2" spans="1:44" s="62" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" s="62" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
         <v>48</v>
       </c>
@@ -5546,11 +5699,8 @@
       <c r="AQ2" s="62" t="s">
         <v>163</v>
       </c>
-      <c r="AR2" s="86" t="s">
-        <v>392</v>
-      </c>
     </row>
-    <row r="3" spans="1:44" s="62" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" s="62" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="71"/>
       <c r="F3" s="63"/>
       <c r="L3" s="63"/>
@@ -5562,7 +5712,7 @@
       <c r="AF3" s="66"/>
       <c r="AH3" s="67"/>
     </row>
-    <row r="4" spans="1:44" s="62" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:43" s="62" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="71"/>
       <c r="F4" s="63"/>
       <c r="L4" s="63"/>
@@ -5574,7 +5724,7 @@
       <c r="AF4" s="66"/>
       <c r="AH4" s="67"/>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="P8" s="70"/>
       <c r="Q8" s="69"/>
     </row>
@@ -5595,8 +5745,8 @@
   </sheetPr>
   <dimension ref="A1:EI3"/>
   <sheetViews>
-    <sheetView topLeftCell="EE1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="EH1" sqref="EH1"/>
+    <sheetView topLeftCell="AK1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AQ11" sqref="AQ11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5735,7 +5885,7 @@
     <col min="137" max="137" width="28" style="86" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:139" s="86" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:139" s="86" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -6987,11 +7137,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:CZ4"/>
+  <dimension ref="A1:CY4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="CU1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CZ1" sqref="CZ1:CZ2"/>
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7000,9 +7150,9 @@
     <col min="2" max="2" width="39.28515625" style="86" customWidth="1"/>
     <col min="3" max="3" width="25.85546875" style="86" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.140625" style="86" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43" style="86" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24" style="86" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" style="86" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" style="86" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" style="86" customWidth="1"/>
     <col min="9" max="9" width="21.85546875" style="86" customWidth="1"/>
     <col min="10" max="11" width="16.85546875" style="86" customWidth="1"/>
@@ -7094,7 +7244,7 @@
     <col min="103" max="103" width="23.42578125" style="78" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:104" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:103" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -7404,11 +7554,8 @@
       <c r="CY1" s="43" t="s">
         <v>451</v>
       </c>
-      <c r="CZ1" s="75" t="s">
-        <v>295</v>
-      </c>
     </row>
-    <row r="2" spans="1:104" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:103" x14ac:dyDescent="0.25">
       <c r="A2" s="46" t="s">
         <v>48</v>
       </c>
@@ -7632,11 +7779,8 @@
       <c r="CW2" s="22" t="s">
         <v>550</v>
       </c>
-      <c r="CZ2" s="86" t="s">
-        <v>392</v>
-      </c>
     </row>
-    <row r="3" spans="1:104" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:103" x14ac:dyDescent="0.25">
       <c r="A3" s="46" t="s">
         <v>394</v>
       </c>
@@ -7728,7 +7872,7 @@
         <v>531</v>
       </c>
       <c r="AE3" s="48" t="s">
-        <v>532</v>
+        <v>552</v>
       </c>
       <c r="AF3" s="48"/>
       <c r="AG3" s="48"/>
@@ -7794,13 +7938,13 @@
         <v>540</v>
       </c>
       <c r="BJ3" t="s">
-        <v>532</v>
+        <v>552</v>
       </c>
       <c r="BL3" t="s">
-        <v>532</v>
+        <v>552</v>
       </c>
       <c r="BN3" t="s">
-        <v>532</v>
+        <v>552</v>
       </c>
       <c r="BO3" s="48"/>
       <c r="BP3" s="48"/>
@@ -7828,13 +7972,13 @@
         <v>300</v>
       </c>
       <c r="CJ3" t="s">
-        <v>532</v>
+        <v>552</v>
       </c>
       <c r="CK3" t="s">
-        <v>532</v>
+        <v>552</v>
       </c>
       <c r="CM3" t="s">
-        <v>532</v>
+        <v>552</v>
       </c>
       <c r="CN3" s="14" t="s">
         <v>519</v>
@@ -7860,13 +8004,10 @@
       <c r="CW3" s="22" t="s">
         <v>550</v>
       </c>
-      <c r="CZ3" s="86" t="s">
-        <v>392</v>
-      </c>
     </row>
-    <row r="4" spans="1:104" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:103" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B4" s="86" t="s">
         <v>512</v>
@@ -7884,7 +8025,7 @@
         <v>516</v>
       </c>
       <c r="G4" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="H4" s="86" t="s">
         <v>310</v>
@@ -7956,7 +8097,7 @@
         <v>531</v>
       </c>
       <c r="AE4" s="48" t="s">
-        <v>532</v>
+        <v>552</v>
       </c>
       <c r="AF4" s="48"/>
       <c r="AG4" s="48"/>
@@ -8022,13 +8163,13 @@
         <v>540</v>
       </c>
       <c r="BJ4" t="s">
-        <v>532</v>
+        <v>552</v>
       </c>
       <c r="BL4" t="s">
-        <v>532</v>
+        <v>552</v>
       </c>
       <c r="BN4" t="s">
-        <v>532</v>
+        <v>552</v>
       </c>
       <c r="BO4" s="48"/>
       <c r="BP4" s="48"/>
@@ -8056,13 +8197,13 @@
         <v>300</v>
       </c>
       <c r="CJ4" t="s">
-        <v>532</v>
+        <v>552</v>
       </c>
       <c r="CK4" t="s">
-        <v>532</v>
+        <v>552</v>
       </c>
       <c r="CM4" t="s">
-        <v>532</v>
+        <v>552</v>
       </c>
       <c r="CN4" s="14" t="s">
         <v>519</v>
@@ -8087,9 +8228,6 @@
       </c>
       <c r="CW4" s="22" t="s">
         <v>550</v>
-      </c>
-      <c r="CZ4" s="86" t="s">
-        <v>392</v>
       </c>
     </row>
   </sheetData>
@@ -8100,22 +8238,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K1" sqref="K1:K2"/>
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.140625" style="86" customWidth="1"/>
     <col min="2" max="2" width="39.28515625" style="86" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.28515625" style="86" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" style="78" customWidth="1"/>
     <col min="5" max="5" width="27.140625" style="78" customWidth="1"/>
     <col min="6" max="6" width="21.140625" style="78" customWidth="1"/>
@@ -8124,7 +8262,7 @@
     <col min="10" max="10" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -8153,13 +8291,10 @@
         <v>451</v>
       </c>
       <c r="J1" s="43" t="s">
-        <v>554</v>
-      </c>
-      <c r="K1" s="75" t="s">
-        <v>295</v>
+        <v>574</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="46" t="s">
         <v>48</v>
       </c>
@@ -8182,13 +8317,10 @@
         <v>48</v>
       </c>
       <c r="I2" s="22" t="s">
-        <v>555</v>
+        <v>575</v>
       </c>
       <c r="J2" t="s">
-        <v>556</v>
-      </c>
-      <c r="K2" s="86" t="s">
-        <v>392</v>
+        <v>576</v>
       </c>
     </row>
   </sheetData>
@@ -8199,17 +8331,17 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AG4"/>
+  <dimension ref="A1:AF4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AF2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AG1" sqref="AG1:AG2"/>
+      <selection pane="bottomRight" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8246,7 +8378,7 @@
     <col min="32" max="32" width="24.42578125" style="86" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="1" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" s="1" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="85" t="s">
         <v>0</v>
       </c>
@@ -8254,10 +8386,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>557</v>
+        <v>577</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>558</v>
+        <v>578</v>
       </c>
       <c r="E1" s="25" t="s">
         <v>419</v>
@@ -8266,99 +8398,96 @@
         <v>421</v>
       </c>
       <c r="G1" s="25" t="s">
-        <v>559</v>
+        <v>579</v>
       </c>
       <c r="H1" s="26" t="s">
         <v>422</v>
       </c>
       <c r="I1" s="26" t="s">
-        <v>560</v>
+        <v>580</v>
       </c>
       <c r="J1" s="26" t="s">
-        <v>561</v>
+        <v>581</v>
       </c>
       <c r="K1" s="26" t="s">
-        <v>562</v>
+        <v>582</v>
       </c>
       <c r="L1" s="26" t="s">
-        <v>563</v>
+        <v>583</v>
       </c>
       <c r="M1" s="25" t="s">
-        <v>564</v>
+        <v>584</v>
       </c>
       <c r="N1" s="25" t="s">
-        <v>565</v>
+        <v>585</v>
       </c>
       <c r="O1" s="25" t="s">
-        <v>566</v>
+        <v>586</v>
       </c>
       <c r="P1" s="25" t="s">
-        <v>567</v>
+        <v>587</v>
       </c>
       <c r="Q1" s="26" t="s">
-        <v>568</v>
+        <v>588</v>
       </c>
       <c r="R1" s="26" t="s">
-        <v>569</v>
+        <v>589</v>
       </c>
       <c r="S1" s="26" t="s">
-        <v>570</v>
+        <v>590</v>
       </c>
       <c r="T1" s="26" t="s">
-        <v>571</v>
+        <v>591</v>
       </c>
       <c r="U1" s="26" t="s">
-        <v>572</v>
+        <v>592</v>
       </c>
       <c r="V1" s="26" t="s">
-        <v>573</v>
+        <v>593</v>
       </c>
       <c r="W1" s="26" t="s">
-        <v>574</v>
+        <v>594</v>
       </c>
       <c r="X1" s="26" t="s">
-        <v>575</v>
+        <v>595</v>
       </c>
       <c r="Y1" s="26" t="s">
-        <v>576</v>
+        <v>596</v>
       </c>
       <c r="Z1" s="26" t="s">
-        <v>577</v>
+        <v>597</v>
       </c>
       <c r="AA1" s="26" t="s">
-        <v>578</v>
+        <v>598</v>
       </c>
       <c r="AB1" s="26" t="s">
-        <v>579</v>
+        <v>599</v>
       </c>
       <c r="AC1" s="25" t="s">
-        <v>580</v>
+        <v>600</v>
       </c>
       <c r="AD1" s="26" t="s">
-        <v>581</v>
+        <v>601</v>
       </c>
       <c r="AE1" s="26" t="s">
-        <v>582</v>
+        <v>602</v>
       </c>
       <c r="AF1" s="26" t="s">
-        <v>583</v>
-      </c>
-      <c r="AG1" s="75" t="s">
-        <v>295</v>
+        <v>603</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="46" t="s">
         <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>584</v>
+        <v>604</v>
       </c>
       <c r="C2" s="46" t="s">
-        <v>585</v>
+        <v>605</v>
       </c>
       <c r="D2" s="86" t="s">
-        <v>586</v>
+        <v>606</v>
       </c>
       <c r="E2" t="s">
         <v>515</v>
@@ -8370,10 +8499,10 @@
         <v>310</v>
       </c>
       <c r="I2" s="86" t="s">
-        <v>587</v>
+        <v>607</v>
       </c>
       <c r="K2" s="84" t="s">
-        <v>588</v>
+        <v>608</v>
       </c>
       <c r="L2" s="86" t="s">
         <v>310</v>
@@ -8385,10 +8514,10 @@
         <v>532</v>
       </c>
       <c r="O2" t="s">
-        <v>589</v>
+        <v>609</v>
       </c>
       <c r="P2" t="s">
-        <v>589</v>
+        <v>609</v>
       </c>
       <c r="R2" s="86" t="s">
         <v>525</v>
@@ -8397,19 +8526,19 @@
         <v>522</v>
       </c>
       <c r="T2" s="22" t="s">
-        <v>590</v>
+        <v>610</v>
       </c>
       <c r="V2" s="86" t="s">
-        <v>591</v>
+        <v>611</v>
       </c>
       <c r="W2" s="86" t="s">
-        <v>592</v>
+        <v>612</v>
       </c>
       <c r="X2" s="86" t="s">
         <v>310</v>
       </c>
       <c r="Z2" s="86" t="s">
-        <v>591</v>
+        <v>611</v>
       </c>
       <c r="AA2" s="86" t="s">
         <v>545</v>
@@ -8421,30 +8550,27 @@
         <v>306</v>
       </c>
       <c r="AD2" s="86" t="s">
-        <v>591</v>
+        <v>611</v>
       </c>
       <c r="AE2" s="86" t="s">
         <v>543</v>
       </c>
       <c r="AF2" s="27" t="s">
-        <v>593</v>
-      </c>
-      <c r="AG2" s="86" t="s">
-        <v>392</v>
+        <v>613</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" s="46" t="s">
         <v>394</v>
       </c>
       <c r="B3" t="s">
-        <v>594</v>
+        <v>614</v>
       </c>
       <c r="C3" s="46" t="s">
-        <v>585</v>
+        <v>605</v>
       </c>
       <c r="D3" s="86" t="s">
-        <v>595</v>
+        <v>615</v>
       </c>
       <c r="E3" t="s">
         <v>515</v>
@@ -8456,10 +8582,10 @@
         <v>310</v>
       </c>
       <c r="I3" s="86" t="s">
-        <v>596</v>
+        <v>616</v>
       </c>
       <c r="K3" s="84" t="s">
-        <v>597</v>
+        <v>617</v>
       </c>
       <c r="L3" s="86" t="s">
         <v>310</v>
@@ -8471,10 +8597,10 @@
         <v>532</v>
       </c>
       <c r="O3" t="s">
-        <v>589</v>
+        <v>609</v>
       </c>
       <c r="P3" t="s">
-        <v>589</v>
+        <v>609</v>
       </c>
       <c r="R3" s="86" t="s">
         <v>525</v>
@@ -8483,19 +8609,19 @@
         <v>522</v>
       </c>
       <c r="T3" s="22" t="s">
-        <v>598</v>
+        <v>618</v>
       </c>
       <c r="V3" s="86" t="s">
-        <v>591</v>
+        <v>611</v>
       </c>
       <c r="W3" s="86" t="s">
-        <v>592</v>
+        <v>612</v>
       </c>
       <c r="X3" s="86" t="s">
         <v>310</v>
       </c>
       <c r="Z3" s="86" t="s">
-        <v>591</v>
+        <v>611</v>
       </c>
       <c r="AA3" s="86" t="s">
         <v>545</v>
@@ -8507,45 +8633,42 @@
         <v>306</v>
       </c>
       <c r="AD3" s="86" t="s">
-        <v>591</v>
+        <v>611</v>
       </c>
       <c r="AE3" s="86" t="s">
         <v>543</v>
       </c>
       <c r="AF3" s="27" t="s">
-        <v>593</v>
-      </c>
-      <c r="AG3" s="86" t="s">
-        <v>392</v>
+        <v>613</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" s="46" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B4" s="86" t="s">
-        <v>599</v>
+        <v>619</v>
       </c>
       <c r="C4" s="46" t="s">
-        <v>585</v>
+        <v>605</v>
       </c>
       <c r="D4" s="86" t="s">
-        <v>600</v>
+        <v>620</v>
       </c>
       <c r="E4" t="s">
         <v>515</v>
       </c>
       <c r="F4" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="H4" s="86" t="s">
         <v>310</v>
       </c>
       <c r="I4" s="86" t="s">
-        <v>596</v>
+        <v>616</v>
       </c>
       <c r="K4" s="84" t="s">
-        <v>601</v>
+        <v>621</v>
       </c>
       <c r="L4" s="86" t="s">
         <v>310</v>
@@ -8557,10 +8680,10 @@
         <v>532</v>
       </c>
       <c r="O4" t="s">
-        <v>589</v>
+        <v>609</v>
       </c>
       <c r="P4" t="s">
-        <v>589</v>
+        <v>609</v>
       </c>
       <c r="R4" s="86" t="s">
         <v>525</v>
@@ -8569,19 +8692,19 @@
         <v>522</v>
       </c>
       <c r="T4" s="22" t="s">
-        <v>598</v>
+        <v>618</v>
       </c>
       <c r="V4" s="86" t="s">
-        <v>591</v>
+        <v>611</v>
       </c>
       <c r="W4" s="86" t="s">
-        <v>592</v>
+        <v>612</v>
       </c>
       <c r="X4" s="86" t="s">
         <v>310</v>
       </c>
       <c r="Z4" s="86" t="s">
-        <v>591</v>
+        <v>611</v>
       </c>
       <c r="AA4" s="86" t="s">
         <v>545</v>
@@ -8593,16 +8716,13 @@
         <v>306</v>
       </c>
       <c r="AD4" s="86" t="s">
-        <v>591</v>
+        <v>611</v>
       </c>
       <c r="AE4" s="86" t="s">
         <v>543</v>
       </c>
       <c r="AF4" s="27" t="s">
-        <v>593</v>
-      </c>
-      <c r="AG4" s="86" t="s">
-        <v>392</v>
+        <v>613</v>
       </c>
     </row>
   </sheetData>
@@ -8613,17 +8733,17 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:V4"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="V1" sqref="V1:V2"/>
+      <selection pane="bottomRight" activeCell="S40" sqref="S40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8648,7 +8768,7 @@
     <col min="21" max="21" width="25.42578125" style="86" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -8659,75 +8779,72 @@
         <v>421</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>602</v>
+        <v>622</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>603</v>
+        <v>623</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>604</v>
+        <v>624</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>605</v>
+        <v>625</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>606</v>
+        <v>626</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>607</v>
+        <v>627</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>608</v>
+        <v>628</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>609</v>
+        <v>629</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>610</v>
+        <v>630</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>611</v>
+        <v>631</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>612</v>
+        <v>632</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>613</v>
+        <v>633</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>614</v>
+        <v>634</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>615</v>
+        <v>635</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>616</v>
+        <v>636</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>617</v>
+        <v>637</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>618</v>
+        <v>638</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>619</v>
-      </c>
-      <c r="V1" s="75" t="s">
-        <v>295</v>
+        <v>639</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="86" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="86" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="86" t="s">
         <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>584</v>
+        <v>604</v>
       </c>
       <c r="C2" s="86" t="s">
         <v>517</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>620</v>
+        <v>640</v>
       </c>
       <c r="E2" s="22" t="s">
         <v>541</v>
@@ -8736,25 +8853,25 @@
         <v>549</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>621</v>
+        <v>641</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>622</v>
+        <v>642</v>
       </c>
       <c r="I2" s="84" t="s">
-        <v>623</v>
+        <v>643</v>
       </c>
       <c r="J2" s="22" t="s">
-        <v>624</v>
+        <v>644</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>555</v>
+        <v>575</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>625</v>
+        <v>645</v>
       </c>
       <c r="M2" s="86" t="s">
-        <v>626</v>
+        <v>646</v>
       </c>
       <c r="N2" s="22" t="s">
         <v>533</v>
@@ -8763,39 +8880,36 @@
         <v>549</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>555</v>
+        <v>575</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>625</v>
+        <v>645</v>
       </c>
       <c r="R2" s="46" t="s">
-        <v>627</v>
+        <v>647</v>
       </c>
       <c r="S2" s="86" t="s">
-        <v>628</v>
+        <v>648</v>
       </c>
       <c r="T2" s="86" t="s">
-        <v>629</v>
+        <v>649</v>
       </c>
       <c r="U2" s="86" t="s">
-        <v>630</v>
-      </c>
-      <c r="V2" s="86" t="s">
-        <v>392</v>
+        <v>650</v>
       </c>
     </row>
-    <row r="3" spans="1:22" s="86" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" s="86" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="46" t="s">
         <v>394</v>
       </c>
       <c r="B3" t="s">
-        <v>594</v>
+        <v>614</v>
       </c>
       <c r="C3" t="s">
         <v>551</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>620</v>
+        <v>640</v>
       </c>
       <c r="E3" s="22" t="s">
         <v>541</v>
@@ -8804,25 +8918,25 @@
         <v>549</v>
       </c>
       <c r="G3" s="22" t="s">
-        <v>621</v>
+        <v>641</v>
       </c>
       <c r="H3" s="22" t="s">
-        <v>622</v>
+        <v>642</v>
       </c>
       <c r="I3" s="84" t="s">
-        <v>623</v>
+        <v>643</v>
       </c>
       <c r="J3" s="22" t="s">
-        <v>624</v>
+        <v>644</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>555</v>
+        <v>575</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>625</v>
+        <v>645</v>
       </c>
       <c r="M3" s="86" t="s">
-        <v>626</v>
+        <v>646</v>
       </c>
       <c r="N3" s="22" t="s">
         <v>533</v>
@@ -8831,39 +8945,36 @@
         <v>549</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>555</v>
+        <v>575</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>625</v>
+        <v>645</v>
       </c>
       <c r="R3" s="46" t="s">
-        <v>627</v>
+        <v>647</v>
       </c>
       <c r="S3" s="86" t="s">
-        <v>628</v>
+        <v>648</v>
       </c>
       <c r="T3" s="86" t="s">
-        <v>629</v>
+        <v>649</v>
       </c>
       <c r="U3" s="86" t="s">
-        <v>630</v>
-      </c>
-      <c r="V3" s="86" t="s">
-        <v>392</v>
+        <v>650</v>
       </c>
     </row>
-    <row r="4" spans="1:22" s="86" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" s="86" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="46" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B4" s="86" t="s">
-        <v>599</v>
+        <v>619</v>
       </c>
       <c r="C4" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>620</v>
+        <v>640</v>
       </c>
       <c r="E4" s="22" t="s">
         <v>541</v>
@@ -8872,25 +8983,25 @@
         <v>549</v>
       </c>
       <c r="G4" s="22" t="s">
-        <v>621</v>
+        <v>641</v>
       </c>
       <c r="H4" s="22" t="s">
-        <v>622</v>
+        <v>642</v>
       </c>
       <c r="I4" s="84" t="s">
-        <v>623</v>
+        <v>643</v>
       </c>
       <c r="J4" s="22" t="s">
-        <v>624</v>
+        <v>644</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>555</v>
+        <v>575</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>625</v>
+        <v>645</v>
       </c>
       <c r="M4" s="86" t="s">
-        <v>626</v>
+        <v>646</v>
       </c>
       <c r="N4" s="22" t="s">
         <v>533</v>
@@ -8899,25 +9010,22 @@
         <v>549</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>555</v>
+        <v>575</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>625</v>
+        <v>645</v>
       </c>
       <c r="R4" s="46" t="s">
-        <v>627</v>
+        <v>647</v>
       </c>
       <c r="S4" s="86" t="s">
-        <v>628</v>
+        <v>648</v>
       </c>
       <c r="T4" s="86" t="s">
-        <v>629</v>
+        <v>649</v>
       </c>
       <c r="U4" s="86" t="s">
-        <v>630</v>
-      </c>
-      <c r="V4" s="86" t="s">
-        <v>392</v>
+        <v>650</v>
       </c>
     </row>
   </sheetData>
@@ -8928,22 +9036,22 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AD4"/>
+  <dimension ref="A1:AC4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="X1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AD1" sqref="AD1:AD4"/>
+      <selection pane="topRight" activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.140625" style="86" customWidth="1"/>
     <col min="2" max="2" width="39.28515625" style="86" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" style="86" customWidth="1"/>
+    <col min="3" max="3" width="46.28515625" style="86" customWidth="1"/>
     <col min="4" max="4" width="34.5703125" style="86" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36.28515625" style="86" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21" style="86" customWidth="1"/>
@@ -8971,7 +9079,7 @@
     <col min="29" max="29" width="31.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -8985,13 +9093,13 @@
         <v>421</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>631</v>
+        <v>651</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>632</v>
+        <v>652</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>633</v>
+        <v>653</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>198</v>
@@ -9000,43 +9108,43 @@
         <v>507</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>634</v>
+        <v>654</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>635</v>
+        <v>655</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>636</v>
+        <v>656</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>637</v>
+        <v>657</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>638</v>
+        <v>658</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>639</v>
+        <v>659</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>640</v>
+        <v>660</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>641</v>
+        <v>661</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>642</v>
+        <v>662</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>643</v>
+        <v>663</v>
       </c>
       <c r="T1" s="51" t="s">
-        <v>644</v>
+        <v>664</v>
       </c>
       <c r="U1" s="51" t="s">
-        <v>645</v>
+        <v>665</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>646</v>
+        <v>666</v>
       </c>
       <c r="W1" s="6" t="s">
         <v>481</v>
@@ -9059,11 +9167,8 @@
       <c r="AC1" s="6" t="s">
         <v>435</v>
       </c>
-      <c r="AD1" s="75" t="s">
-        <v>295</v>
-      </c>
     </row>
-    <row r="2" spans="1:30" s="86" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="86" t="s">
         <v>48</v>
       </c>
@@ -9086,10 +9191,10 @@
         <v>528</v>
       </c>
       <c r="H2" s="86" t="s">
-        <v>647</v>
+        <v>667</v>
       </c>
       <c r="I2" s="86" t="s">
-        <v>648</v>
+        <v>668</v>
       </c>
       <c r="J2" s="86">
         <v>100</v>
@@ -9098,10 +9203,10 @@
         <v>100</v>
       </c>
       <c r="L2" s="46" t="s">
-        <v>588</v>
+        <v>608</v>
       </c>
       <c r="M2" s="86" t="s">
-        <v>649</v>
+        <v>669</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>524</v>
@@ -9110,19 +9215,19 @@
         <v>525</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>650</v>
+        <v>670</v>
       </c>
       <c r="Q2" s="86" t="s">
         <v>545</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>651</v>
+        <v>671</v>
       </c>
       <c r="S2" s="5" t="s">
         <v>368</v>
       </c>
       <c r="T2" s="86" t="s">
-        <v>589</v>
+        <v>609</v>
       </c>
       <c r="U2" s="86" t="s">
         <v>532</v>
@@ -9131,7 +9236,7 @@
         <v>545</v>
       </c>
       <c r="X2" s="14" t="s">
-        <v>651</v>
+        <v>671</v>
       </c>
       <c r="Y2" s="86" t="s">
         <v>532</v>
@@ -9148,11 +9253,8 @@
       <c r="AC2" s="86" t="s">
         <v>525</v>
       </c>
-      <c r="AD2" s="86" t="s">
-        <v>392</v>
-      </c>
     </row>
-    <row r="3" spans="1:30" s="86" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="46" t="s">
         <v>394</v>
       </c>
@@ -9175,10 +9277,10 @@
         <v>528</v>
       </c>
       <c r="H3" s="86" t="s">
-        <v>647</v>
+        <v>667</v>
       </c>
       <c r="I3" s="86" t="s">
-        <v>648</v>
+        <v>668</v>
       </c>
       <c r="J3" s="86">
         <v>100</v>
@@ -9187,10 +9289,10 @@
         <v>100</v>
       </c>
       <c r="L3" s="46" t="s">
-        <v>597</v>
+        <v>617</v>
       </c>
       <c r="M3" s="86" t="s">
-        <v>649</v>
+        <v>669</v>
       </c>
       <c r="N3" s="5" t="s">
         <v>524</v>
@@ -9199,34 +9301,34 @@
         <v>525</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>650</v>
+        <v>670</v>
       </c>
       <c r="Q3" s="86" t="s">
         <v>545</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>651</v>
+        <v>671</v>
       </c>
       <c r="S3" s="5" t="s">
         <v>368</v>
       </c>
       <c r="T3" s="86" t="s">
-        <v>589</v>
+        <v>609</v>
       </c>
       <c r="U3" s="86" t="s">
-        <v>532</v>
+        <v>552</v>
       </c>
       <c r="W3" s="86" t="s">
         <v>545</v>
       </c>
       <c r="X3" s="14" t="s">
-        <v>651</v>
+        <v>671</v>
       </c>
       <c r="Y3" s="86" t="s">
-        <v>532</v>
+        <v>552</v>
       </c>
       <c r="Z3" s="86" t="s">
-        <v>532</v>
+        <v>552</v>
       </c>
       <c r="AA3" s="86" t="s">
         <v>522</v>
@@ -9237,13 +9339,10 @@
       <c r="AC3" s="86" t="s">
         <v>525</v>
       </c>
-      <c r="AD3" s="86" t="s">
-        <v>392</v>
-      </c>
     </row>
-    <row r="4" spans="1:30" s="86" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B4" s="86" t="s">
         <v>512</v>
@@ -9252,7 +9351,7 @@
         <v>515</v>
       </c>
       <c r="D4" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="E4" s="86" t="s">
         <v>522</v>
@@ -9264,10 +9363,10 @@
         <v>528</v>
       </c>
       <c r="H4" s="86" t="s">
-        <v>647</v>
+        <v>667</v>
       </c>
       <c r="I4" s="86" t="s">
-        <v>648</v>
+        <v>668</v>
       </c>
       <c r="J4" s="86">
         <v>100</v>
@@ -9276,10 +9375,10 @@
         <v>100</v>
       </c>
       <c r="L4" s="46" t="s">
-        <v>601</v>
+        <v>621</v>
       </c>
       <c r="M4" s="86" t="s">
-        <v>649</v>
+        <v>669</v>
       </c>
       <c r="N4" s="5" t="s">
         <v>524</v>
@@ -9288,34 +9387,34 @@
         <v>525</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>650</v>
+        <v>670</v>
       </c>
       <c r="Q4" s="86" t="s">
         <v>545</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>651</v>
+        <v>671</v>
       </c>
       <c r="S4" s="5" t="s">
         <v>368</v>
       </c>
       <c r="T4" s="86" t="s">
-        <v>589</v>
+        <v>609</v>
       </c>
       <c r="U4" s="86" t="s">
-        <v>532</v>
+        <v>552</v>
       </c>
       <c r="W4" s="86" t="s">
         <v>545</v>
       </c>
       <c r="X4" s="14" t="s">
-        <v>651</v>
+        <v>671</v>
       </c>
       <c r="Y4" s="86" t="s">
-        <v>532</v>
+        <v>552</v>
       </c>
       <c r="Z4" s="86" t="s">
-        <v>532</v>
+        <v>552</v>
       </c>
       <c r="AA4" s="86" t="s">
         <v>522</v>
@@ -9325,9 +9424,6 @@
       </c>
       <c r="AC4" s="86" t="s">
         <v>525</v>
-      </c>
-      <c r="AD4" s="86" t="s">
-        <v>392</v>
       </c>
     </row>
   </sheetData>
@@ -9338,14 +9434,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AS5"/>
+  <dimension ref="A1:AR5"/>
   <sheetViews>
-    <sheetView topLeftCell="AJ1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AS1" sqref="AS1:AS2"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9395,7 +9491,7 @@
     <col min="44" max="44" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
@@ -9409,91 +9505,91 @@
         <v>419</v>
       </c>
       <c r="E1" s="29" t="s">
-        <v>563</v>
+        <v>583</v>
       </c>
       <c r="F1" s="30" t="s">
         <v>421</v>
       </c>
       <c r="G1" s="29" t="s">
-        <v>652</v>
+        <v>672</v>
       </c>
       <c r="H1" s="29" t="s">
-        <v>653</v>
+        <v>673</v>
       </c>
       <c r="I1" s="29" t="s">
-        <v>654</v>
+        <v>674</v>
       </c>
       <c r="J1" s="30" t="s">
         <v>426</v>
       </c>
       <c r="K1" s="29" t="s">
-        <v>655</v>
+        <v>675</v>
       </c>
       <c r="L1" s="30" t="s">
-        <v>656</v>
+        <v>676</v>
       </c>
       <c r="M1" s="30" t="s">
-        <v>657</v>
+        <v>677</v>
       </c>
       <c r="N1" s="29" t="s">
-        <v>658</v>
+        <v>678</v>
       </c>
       <c r="O1" s="29" t="s">
-        <v>659</v>
+        <v>679</v>
       </c>
       <c r="P1" s="29" t="s">
-        <v>660</v>
+        <v>680</v>
       </c>
       <c r="Q1" s="29" t="s">
-        <v>661</v>
+        <v>681</v>
       </c>
       <c r="R1" s="30" t="s">
-        <v>662</v>
+        <v>682</v>
       </c>
       <c r="S1" s="30" t="s">
-        <v>663</v>
+        <v>683</v>
       </c>
       <c r="T1" s="29" t="s">
-        <v>664</v>
+        <v>684</v>
       </c>
       <c r="U1" s="29" t="s">
-        <v>665</v>
+        <v>685</v>
       </c>
       <c r="V1" s="29" t="s">
-        <v>666</v>
+        <v>686</v>
       </c>
       <c r="W1" s="29" t="s">
-        <v>667</v>
+        <v>687</v>
       </c>
       <c r="X1" s="29" t="s">
-        <v>668</v>
+        <v>688</v>
       </c>
       <c r="Y1" s="29" t="s">
-        <v>669</v>
+        <v>689</v>
       </c>
       <c r="Z1" s="30" t="s">
-        <v>670</v>
+        <v>690</v>
       </c>
       <c r="AA1" s="29" t="s">
-        <v>671</v>
+        <v>691</v>
       </c>
       <c r="AB1" s="2" t="s">
-        <v>672</v>
+        <v>692</v>
       </c>
       <c r="AC1" s="2" t="s">
-        <v>673</v>
+        <v>693</v>
       </c>
       <c r="AD1" s="2" t="s">
-        <v>674</v>
+        <v>694</v>
       </c>
       <c r="AE1" s="2" t="s">
-        <v>675</v>
+        <v>695</v>
       </c>
       <c r="AF1" s="2" t="s">
-        <v>676</v>
+        <v>696</v>
       </c>
       <c r="AG1" s="2" t="s">
-        <v>677</v>
+        <v>697</v>
       </c>
       <c r="AH1" s="13" t="s">
         <v>174</v>
@@ -9505,34 +9601,31 @@
         <v>166</v>
       </c>
       <c r="AK1" s="2" t="s">
-        <v>678</v>
+        <v>698</v>
       </c>
       <c r="AL1" s="2" t="s">
-        <v>659</v>
+        <v>679</v>
       </c>
       <c r="AM1" s="13" t="s">
-        <v>679</v>
+        <v>699</v>
       </c>
       <c r="AN1" s="2" t="s">
-        <v>680</v>
+        <v>700</v>
       </c>
       <c r="AO1" s="2" t="s">
-        <v>681</v>
+        <v>701</v>
       </c>
       <c r="AP1" s="2" t="s">
-        <v>682</v>
+        <v>702</v>
       </c>
       <c r="AQ1" s="2" t="s">
-        <v>683</v>
+        <v>703</v>
       </c>
       <c r="AR1" s="2" t="s">
-        <v>684</v>
-      </c>
-      <c r="AS1" s="75" t="s">
-        <v>295</v>
+        <v>704</v>
       </c>
     </row>
-    <row r="2" spans="1:45" s="86" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="86" t="s">
         <v>48</v>
       </c>
@@ -9549,37 +9642,37 @@
         <v>310</v>
       </c>
       <c r="F2" s="86" t="s">
-        <v>685</v>
+        <v>705</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>628</v>
+        <v>648</v>
       </c>
       <c r="H2" s="86" t="s">
-        <v>651</v>
+        <v>671</v>
       </c>
       <c r="I2" s="86" t="s">
-        <v>686</v>
+        <v>706</v>
       </c>
       <c r="J2" s="86" t="s">
         <v>306</v>
       </c>
       <c r="K2" s="15" t="s">
-        <v>598</v>
+        <v>618</v>
       </c>
       <c r="L2" s="86" t="s">
-        <v>685</v>
+        <v>705</v>
       </c>
       <c r="M2" s="86" t="s">
-        <v>687</v>
+        <v>707</v>
       </c>
       <c r="N2" s="15" t="s">
-        <v>630</v>
+        <v>650</v>
       </c>
       <c r="O2" s="15" t="s">
         <v>310</v>
       </c>
       <c r="P2" s="15" t="s">
-        <v>688</v>
+        <v>708</v>
       </c>
       <c r="Q2" s="15" t="s">
         <v>368</v>
@@ -9588,22 +9681,22 @@
         <v>532</v>
       </c>
       <c r="S2" s="86" t="s">
-        <v>589</v>
+        <v>709</v>
       </c>
       <c r="T2" s="15" t="s">
-        <v>689</v>
+        <v>710</v>
       </c>
       <c r="U2" s="15" t="s">
-        <v>689</v>
+        <v>710</v>
       </c>
       <c r="V2" s="15" t="s">
-        <v>690</v>
+        <v>711</v>
       </c>
       <c r="W2" s="15" t="s">
-        <v>691</v>
+        <v>712</v>
       </c>
       <c r="X2" s="15" t="s">
-        <v>692</v>
+        <v>713</v>
       </c>
       <c r="Y2" s="15" t="s">
         <v>48</v>
@@ -9612,22 +9705,22 @@
         <v>532</v>
       </c>
       <c r="AA2" s="15" t="s">
-        <v>693</v>
+        <v>714</v>
       </c>
       <c r="AB2" s="86" t="s">
-        <v>694</v>
+        <v>715</v>
       </c>
       <c r="AC2" s="86" t="s">
-        <v>695</v>
+        <v>567</v>
       </c>
       <c r="AD2" s="86" t="s">
-        <v>696</v>
+        <v>716</v>
       </c>
       <c r="AE2" s="15" t="s">
-        <v>697</v>
+        <v>717</v>
       </c>
       <c r="AF2" s="15" t="s">
-        <v>698</v>
+        <v>718</v>
       </c>
       <c r="AG2" s="15" t="s">
         <v>322</v>
@@ -9636,13 +9729,13 @@
         <v>306</v>
       </c>
       <c r="AI2" s="86" t="s">
-        <v>699</v>
+        <v>719</v>
       </c>
       <c r="AJ2" s="86" t="s">
         <v>300</v>
       </c>
       <c r="AK2" s="86" t="s">
-        <v>700</v>
+        <v>720</v>
       </c>
       <c r="AL2" s="86" t="s">
         <v>310</v>
@@ -9651,31 +9744,22 @@
         <v>308</v>
       </c>
       <c r="AN2" s="32" t="s">
-        <v>701</v>
+        <v>721</v>
       </c>
       <c r="AO2" s="32" t="s">
-        <v>702</v>
+        <v>722</v>
       </c>
       <c r="AP2" s="86" t="s">
-        <v>703</v>
+        <v>723</v>
       </c>
       <c r="AQ2" s="86" t="s">
-        <v>704</v>
+        <v>724</v>
       </c>
       <c r="AR2" s="86" t="s">
-        <v>705</v>
-      </c>
-      <c r="AS2" s="86" t="s">
-        <v>392</v>
+        <v>725</v>
       </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="AS3" s="86"/>
-    </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="AS4" s="86"/>
-    </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="AP5" s="33"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feature/GDE-8189 RPA Scenario 1 comprehensive repricing updates
Added new keyword for RPA scenario 1
Updated test suite and data set
Added global variable
Updated keyword for writing on comprehensive repricing sheet
Updated loan drawdown keyword on test suite
</commit_message>
<xml_diff>
--- a/DataSet/LoanIQ_DataSet/EU_Entity/EVG_S1_EU_RPA_InternalDeal.xlsx
+++ b/DataSet/LoanIQ_DataSet/EU_Entity/EVG_S1_EU_RPA_InternalDeal.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="7" activeTab="10" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="7" activeTab="12" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
@@ -18,12 +18,13 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TRPO12_PortfolioSettledDisc" sheetId="10" state="visible" r:id="rId10"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TRPO06_InternalParticipation" sheetId="11" state="visible" r:id="rId11"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV01_LoanDrawdown" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AMCH06_PricingChangeTransaction" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DLCH01_DealChangeTransaction" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV18_Payments" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV21_InterestPayments" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV29_PaymentFees" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AMCH04_DealChangeTransaction" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV08_ComprehensiveRepricing" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AMCH06_PricingChangeTransaction" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DLCH01_DealChangeTransaction" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV18_Payments" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV21_InterestPayments" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV29_PaymentFees" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AMCH04_DealChangeTransaction" sheetId="19" state="visible" r:id="rId19"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -36,7 +37,7 @@
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="m/d/yy"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="24">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -175,8 +176,19 @@
       <color rgb="FFFF0000"/>
       <sz val="11"/>
     </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <sz val="12"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill/>
     </fill>
@@ -240,6 +252,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.09997863704336681"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -315,12 +333,12 @@
     </border>
   </borders>
   <cellStyleXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -467,6 +485,33 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="13" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="23" fillId="2" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="23" fillId="3" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="12" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="4" fillId="12" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1423,29 +1468,29 @@
   </sheetPr>
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="U42" sqref="U42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col width="5.85546875" bestFit="1" customWidth="1" style="92" min="1" max="1"/>
-    <col width="28" bestFit="1" customWidth="1" style="92" min="2" max="2"/>
-    <col width="44" bestFit="1" customWidth="1" style="92" min="3" max="3"/>
-    <col width="32.28515625" bestFit="1" customWidth="1" style="92" min="4" max="4"/>
-    <col width="21.7109375" customWidth="1" style="92" min="5" max="6"/>
-    <col width="36.7109375" bestFit="1" customWidth="1" style="92" min="7" max="7"/>
-    <col width="36.7109375" customWidth="1" style="92" min="8" max="8"/>
-    <col width="35.7109375" bestFit="1" customWidth="1" style="92" min="9" max="9"/>
-    <col width="32.28515625" bestFit="1" customWidth="1" style="92" min="10" max="10"/>
-    <col width="17" bestFit="1" customWidth="1" style="92" min="11" max="11"/>
-    <col width="24.28515625" bestFit="1" customWidth="1" style="92" min="12" max="12"/>
-    <col width="44.28515625" bestFit="1" customWidth="1" style="92" min="13" max="13"/>
-    <col width="23.42578125" bestFit="1" customWidth="1" style="92" min="14" max="14"/>
-    <col width="32.7109375" bestFit="1" customWidth="1" style="92" min="15" max="15"/>
-    <col width="12.28515625" bestFit="1" customWidth="1" style="92" min="16" max="16"/>
-    <col width="8.7109375" customWidth="1" style="92" min="17" max="42"/>
-    <col width="8.7109375" customWidth="1" style="92" min="43" max="16384"/>
+    <col width="5.85546875" bestFit="1" customWidth="1" style="116" min="1" max="1"/>
+    <col width="28" bestFit="1" customWidth="1" style="116" min="2" max="2"/>
+    <col width="44" bestFit="1" customWidth="1" style="116" min="3" max="3"/>
+    <col width="32.28515625" bestFit="1" customWidth="1" style="116" min="4" max="4"/>
+    <col width="21.7109375" customWidth="1" style="116" min="5" max="6"/>
+    <col width="36.7109375" bestFit="1" customWidth="1" style="116" min="7" max="7"/>
+    <col width="36.7109375" customWidth="1" style="116" min="8" max="8"/>
+    <col width="35.7109375" bestFit="1" customWidth="1" style="116" min="9" max="9"/>
+    <col width="32.28515625" bestFit="1" customWidth="1" style="116" min="10" max="10"/>
+    <col width="17" bestFit="1" customWidth="1" style="116" min="11" max="11"/>
+    <col width="24.28515625" bestFit="1" customWidth="1" style="116" min="12" max="12"/>
+    <col width="44.28515625" bestFit="1" customWidth="1" style="116" min="13" max="13"/>
+    <col width="23.42578125" bestFit="1" customWidth="1" style="116" min="14" max="14"/>
+    <col width="32.7109375" bestFit="1" customWidth="1" style="116" min="15" max="15"/>
+    <col width="12.28515625" bestFit="1" customWidth="1" style="116" min="16" max="16"/>
+    <col width="8.7109375" customWidth="1" style="116" min="17" max="48"/>
+    <col width="8.7109375" customWidth="1" style="116" min="49" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="87">
@@ -1541,14 +1586,14 @@
           <t>EVG_S1_EU_RPA_InternalDeal</t>
         </is>
       </c>
-      <c r="C2" s="92" t="inlineStr">
-        <is>
-          <t>RPA INTERNAL 100M EURO30102020121245TGJ</t>
+      <c r="C2" s="116" t="inlineStr">
+        <is>
+          <t>RPA INTERNAL 100M EURO04112020090259OJX</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>INTFULDRAW30102020122129DGS</t>
+          <t>INTFULDRAW04112020091041ZVV</t>
         </is>
       </c>
       <c r="E2" s="93" t="inlineStr">
@@ -1578,7 +1623,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>INTFULDRAW30102020122129DGS</t>
+          <t>INTFULDRAW04112020091041ZVV</t>
         </is>
       </c>
       <c r="K2" s="91" t="n">
@@ -1589,24 +1634,24 @@
           <t>Fees Held Awaiting Dispos.</t>
         </is>
       </c>
-      <c r="M2" s="92" t="inlineStr">
-        <is>
-          <t>RPA INTERNAL 100M EURO30102020121245TGJ</t>
-        </is>
-      </c>
-      <c r="N2" s="92" t="inlineStr">
+      <c r="M2" s="116" t="inlineStr">
+        <is>
+          <t>RPA INTERNAL 100M EURO04112020090259OJX</t>
+        </is>
+      </c>
+      <c r="N2" s="116" t="inlineStr">
         <is>
           <t>Facilities</t>
         </is>
       </c>
-      <c r="O2" s="92" t="inlineStr">
+      <c r="O2" s="116" t="inlineStr">
         <is>
           <t>Portfolio Settled Discount Adjustment</t>
         </is>
       </c>
       <c r="P2" s="103" t="inlineStr">
         <is>
-          <t>10-Aug-2020</t>
+          <t>03-Nov-2020</t>
         </is>
       </c>
     </row>
@@ -1625,8 +1670,8 @@
   </sheetPr>
   <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -1785,12 +1830,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>RPA INTERNAL 100M EURO30102020121245TGJ</t>
+          <t>RPA INTERNAL 100M EURO04112020090259OJX</t>
         </is>
       </c>
       <c r="D2" s="93" t="inlineStr">
         <is>
-          <t>INTFULDRAW30102020122129DGS</t>
+          <t>INTFULDRAW04112020091041ZVV</t>
         </is>
       </c>
       <c r="E2" s="93" t="inlineStr">
@@ -1842,7 +1887,7 @@
       </c>
       <c r="P2" s="11" t="inlineStr">
         <is>
-          <t>10-Aug-2020</t>
+          <t>03-Nov-2020</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
@@ -1860,12 +1905,12 @@
           <t>Awaiting Complete Portfolio Allocations</t>
         </is>
       </c>
-      <c r="T2" s="92" t="inlineStr">
+      <c r="T2" s="116" t="inlineStr">
         <is>
           <t>Circles</t>
         </is>
       </c>
-      <c r="U2" s="92" t="inlineStr">
+      <c r="U2" s="116" t="inlineStr">
         <is>
           <t>Hold for Investment - Australia</t>
         </is>
@@ -1894,7 +1939,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>PARDRAW30102020123027LKM</t>
+          <t>PARDRAW04112020091859TQL</t>
         </is>
       </c>
       <c r="L3" t="n">
@@ -1914,7 +1959,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>INTUND30102020123930CUQ</t>
+          <t>INTUND04112020092726MHD</t>
         </is>
       </c>
       <c r="L4" t="n">
@@ -1936,8 +1981,8 @@
   </sheetPr>
   <dimension ref="A1:AR5"/>
   <sheetViews>
-    <sheetView topLeftCell="AI1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AO3" sqref="AO3"/>
+    <sheetView topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -2224,9 +2269,9 @@
           <t>john.blogg@abc.com</t>
         </is>
       </c>
-      <c r="D2" s="92" t="inlineStr">
-        <is>
-          <t>RPA INTERNAL 100M EURO30102020121245TGJ</t>
+      <c r="D2" s="116" t="inlineStr">
+        <is>
+          <t>RPA INTERNAL 100M EURO04112020090259OJX</t>
         </is>
       </c>
       <c r="E2" s="15" t="inlineStr">
@@ -2236,13 +2281,11 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>INTFULDRAW30102020122129DGS</t>
-        </is>
-      </c>
-      <c r="G2" s="15" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+          <t>INTFULDRAW04112020091041ZVV</t>
+        </is>
+      </c>
+      <c r="G2" s="15" t="n">
+        <v>2.5</v>
       </c>
       <c r="H2" s="93" t="inlineStr">
         <is>
@@ -2266,12 +2309,12 @@
       </c>
       <c r="L2" s="93" t="inlineStr">
         <is>
-          <t>INTFULDRAW30102020122129DGS</t>
+          <t>INTFULDRAW04112020091041ZVV</t>
         </is>
       </c>
       <c r="M2" s="93" t="inlineStr">
         <is>
-          <t>60000485</t>
+          <t>60000715</t>
         </is>
       </c>
       <c r="N2" s="15" t="inlineStr">
@@ -2289,12 +2332,12 @@
       </c>
       <c r="Q2" s="93" t="inlineStr">
         <is>
-          <t>10-Aug-2020</t>
+          <t>03-Nov-2020</t>
         </is>
       </c>
       <c r="R2" s="93" t="inlineStr">
         <is>
-          <t>11-Aug-2025</t>
+          <t>03-Nov-2025</t>
         </is>
       </c>
       <c r="S2" s="15" t="inlineStr">
@@ -2329,7 +2372,7 @@
       </c>
       <c r="Y2" s="93" t="inlineStr">
         <is>
-          <t>10-Aug-2020</t>
+          <t>03-Nov-2020</t>
         </is>
       </c>
       <c r="Z2" s="15" t="inlineStr">
@@ -2409,7 +2452,7 @@
       </c>
       <c r="AO2" s="52" t="inlineStr">
         <is>
-          <t>CG852/Hold for Investment - Europe/IT_SAF</t>
+          <t>CB022/Hold for Investment - Australia/DM_CFS</t>
         </is>
       </c>
       <c r="AP2" s="93" t="inlineStr">
@@ -2417,9 +2460,9 @@
           <t>Awaiting release</t>
         </is>
       </c>
-      <c r="AQ2" s="93" t="inlineStr">
-        <is>
-          <t>CG852</t>
+      <c r="AQ2" s="52" t="inlineStr">
+        <is>
+          <t>CB022</t>
         </is>
       </c>
       <c r="AR2" s="93" t="inlineStr">
@@ -2444,9 +2487,9 @@
           <t>john.blogg@abc.com</t>
         </is>
       </c>
-      <c r="D3" s="92" t="inlineStr">
-        <is>
-          <t>RPA INTERNAL 100M EURO30102020121245TGJ</t>
+      <c r="D3" s="116" t="inlineStr">
+        <is>
+          <t>RPA INTERNAL 100M EURO04112020090259OJX</t>
         </is>
       </c>
       <c r="E3" s="15" t="inlineStr">
@@ -2456,13 +2499,11 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>PARDRAW30102020123027LKM</t>
-        </is>
-      </c>
-      <c r="G3" s="15" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+          <t>PARDRAW04112020091859TQL</t>
+        </is>
+      </c>
+      <c r="G3" s="15" t="n">
+        <v>2.5</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -2486,12 +2527,12 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>PARDRAW30102020123027LKM</t>
+          <t>PARDRAW04112020091859TQL</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>60000486</t>
+          <t>60000716</t>
         </is>
       </c>
       <c r="N3" s="15" t="inlineStr">
@@ -2509,12 +2550,12 @@
       </c>
       <c r="Q3" s="93" t="inlineStr">
         <is>
-          <t>10-Aug-2020</t>
+          <t>03-Nov-2020</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>11-Aug-2025</t>
+          <t>03-Nov-2025</t>
         </is>
       </c>
       <c r="S3" s="15" t="inlineStr">
@@ -2549,7 +2590,7 @@
       </c>
       <c r="Y3" s="93" t="inlineStr">
         <is>
-          <t>10-Aug-2020</t>
+          <t>03-Nov-2020</t>
         </is>
       </c>
       <c r="Z3" s="15" t="inlineStr">
@@ -2624,7 +2665,7 @@
       </c>
       <c r="AO3" s="52" t="inlineStr">
         <is>
-          <t>CG852/Hold for Investment - Europe/IT_SAF</t>
+          <t>CB022/Hold for Investment - Australia/DM_CFS</t>
         </is>
       </c>
       <c r="AP3" s="93" t="inlineStr">
@@ -2632,9 +2673,9 @@
           <t>Awaiting release</t>
         </is>
       </c>
-      <c r="AQ3" s="93" t="inlineStr">
-        <is>
-          <t>CG852</t>
+      <c r="AQ3" s="52" t="inlineStr">
+        <is>
+          <t>CB022</t>
         </is>
       </c>
     </row>
@@ -2650,25 +2691,25 @@
         </is>
       </c>
       <c r="C4" s="31" t="n"/>
-      <c r="D4" s="92" t="n"/>
+      <c r="D4" s="116" t="n"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>INTUND30102020123930CUQ</t>
+          <t>INTUND04112020092726MHD</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>INTUND30102020123930CUQ</t>
+          <t>INTUND04112020092726MHD</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>10-Aug-2020</t>
+          <t>03-Nov-2020</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>11-Aug-2025</t>
+          <t>03-Nov-2025</t>
         </is>
       </c>
     </row>
@@ -2685,13 +2726,514 @@
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AN4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AM2" sqref="AM2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
+  <cols>
+    <col width="6.85546875" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="50.140625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="43.7109375" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="26.140625" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="31.5703125" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="17.7109375" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="22.28515625" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="16.42578125" bestFit="1" customWidth="1" min="8" max="8"/>
+    <col width="24.140625" bestFit="1" customWidth="1" min="9" max="9"/>
+    <col width="31.5703125" bestFit="1" customWidth="1" min="10" max="10"/>
+    <col width="16" bestFit="1" customWidth="1" min="11" max="11"/>
+    <col width="23.5703125" bestFit="1" customWidth="1" min="12" max="12"/>
+    <col width="31.42578125" bestFit="1" customWidth="1" min="13" max="13"/>
+    <col width="22.140625" bestFit="1" customWidth="1" min="14" max="14"/>
+    <col width="25.140625" bestFit="1" customWidth="1" min="15" max="15"/>
+    <col width="25.140625" customWidth="1" min="16" max="16"/>
+    <col width="26.5703125" bestFit="1" customWidth="1" min="17" max="17"/>
+    <col width="25.5703125" bestFit="1" customWidth="1" min="18" max="18"/>
+    <col width="25.5703125" customWidth="1" min="19" max="19"/>
+    <col width="26.85546875" bestFit="1" customWidth="1" min="20" max="20"/>
+    <col width="26.7109375" bestFit="1" customWidth="1" min="21" max="21"/>
+    <col width="16.28515625" bestFit="1" customWidth="1" min="22" max="22"/>
+    <col width="20.28515625" bestFit="1" customWidth="1" min="23" max="23"/>
+    <col width="11.5703125" bestFit="1" customWidth="1" min="24" max="24"/>
+    <col width="20.28515625" bestFit="1" customWidth="1" min="25" max="25"/>
+    <col width="19.85546875" bestFit="1" customWidth="1" min="26" max="26"/>
+    <col width="22.28515625" bestFit="1" customWidth="1" min="27" max="27"/>
+    <col width="21.85546875" bestFit="1" customWidth="1" min="28" max="29"/>
+    <col width="21.140625" bestFit="1" customWidth="1" min="30" max="30"/>
+    <col width="24.28515625" bestFit="1" customWidth="1" min="31" max="31"/>
+    <col width="15.140625" bestFit="1" customWidth="1" min="32" max="32"/>
+    <col width="20" bestFit="1" customWidth="1" min="33" max="33"/>
+    <col width="17.28515625" bestFit="1" customWidth="1" min="34" max="35"/>
+    <col width="39.42578125" bestFit="1" customWidth="1" min="36" max="36"/>
+    <col width="19" bestFit="1" customWidth="1" min="37" max="37"/>
+    <col width="22.42578125" bestFit="1" customWidth="1" min="38" max="38"/>
+    <col width="19" bestFit="1" customWidth="1" min="39" max="39"/>
+    <col width="24.85546875" bestFit="1" customWidth="1" min="40" max="40"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="16.5" customFormat="1" customHeight="1" s="107" thickBot="1">
+      <c r="A1" s="107" t="inlineStr">
+        <is>
+          <t>rowid</t>
+        </is>
+      </c>
+      <c r="B1" s="107" t="inlineStr">
+        <is>
+          <t>Test_Case</t>
+        </is>
+      </c>
+      <c r="C1" s="108" t="inlineStr">
+        <is>
+          <t>Deal_Name</t>
+        </is>
+      </c>
+      <c r="D1" s="107" t="inlineStr">
+        <is>
+          <t>OutstandingSelect_Type</t>
+        </is>
+      </c>
+      <c r="E1" s="108" t="inlineStr">
+        <is>
+          <t>Facility_Name</t>
+        </is>
+      </c>
+      <c r="F1" s="108" t="inlineStr">
+        <is>
+          <t>Loan_Alias</t>
+        </is>
+      </c>
+      <c r="G1" s="107" t="inlineStr">
+        <is>
+          <t>Repricing_Type</t>
+        </is>
+      </c>
+      <c r="H1" s="108" t="inlineStr">
+        <is>
+          <t>Repricing_Date</t>
+        </is>
+      </c>
+      <c r="I1" s="107" t="inlineStr">
+        <is>
+          <t>Repricing_Add_Option</t>
+        </is>
+      </c>
+      <c r="J1" s="107" t="inlineStr">
+        <is>
+          <t>Repricing_Add_Option_Setup</t>
+        </is>
+      </c>
+      <c r="K1" s="107" t="inlineStr">
+        <is>
+          <t>Pricing_Option</t>
+        </is>
+      </c>
+      <c r="L1" s="109" t="inlineStr">
+        <is>
+          <t>Borrower_ShortName</t>
+        </is>
+      </c>
+      <c r="M1" s="109" t="inlineStr">
+        <is>
+          <t>Lender1_ShortName</t>
+        </is>
+      </c>
+      <c r="N1" s="109" t="inlineStr">
+        <is>
+          <t>Lender2_ShortName</t>
+        </is>
+      </c>
+      <c r="O1" s="108" t="inlineStr">
+        <is>
+          <t>Remittance_Instruction</t>
+        </is>
+      </c>
+      <c r="P1" s="108" t="inlineStr">
+        <is>
+          <t>Remittance1_Instruction</t>
+        </is>
+      </c>
+      <c r="Q1" s="108" t="inlineStr">
+        <is>
+          <t>Remittance2_Instruction</t>
+        </is>
+      </c>
+      <c r="R1" s="108" t="inlineStr">
+        <is>
+          <t>Remittance_Description</t>
+        </is>
+      </c>
+      <c r="S1" s="108" t="inlineStr">
+        <is>
+          <t>Remittance1_Description</t>
+        </is>
+      </c>
+      <c r="T1" s="108" t="inlineStr">
+        <is>
+          <t>Remittance2_Description</t>
+        </is>
+      </c>
+      <c r="U1" s="108" t="inlineStr">
+        <is>
+          <t>Loan_RequestedAmount</t>
+        </is>
+      </c>
+      <c r="V1" s="107" t="inlineStr">
+        <is>
+          <t>Loan_Currency</t>
+        </is>
+      </c>
+      <c r="W1" s="107" t="inlineStr">
+        <is>
+          <t>Remittance_Status</t>
+        </is>
+      </c>
+      <c r="X1" s="107" t="inlineStr">
+        <is>
+          <t>Base_Rate</t>
+        </is>
+      </c>
+      <c r="Y1" s="107" t="inlineStr">
+        <is>
+          <t>Original_Username</t>
+        </is>
+      </c>
+      <c r="Z1" s="107" t="inlineStr">
+        <is>
+          <t>Original_Password</t>
+        </is>
+      </c>
+      <c r="AA1" s="107" t="inlineStr">
+        <is>
+          <t>Approver_Username</t>
+        </is>
+      </c>
+      <c r="AB1" s="107" t="inlineStr">
+        <is>
+          <t>Approver_Password</t>
+        </is>
+      </c>
+      <c r="AC1" s="107" t="inlineStr">
+        <is>
+          <t>Manager_Username</t>
+        </is>
+      </c>
+      <c r="AD1" s="107" t="inlineStr">
+        <is>
+          <t>Manager_Password</t>
+        </is>
+      </c>
+      <c r="AE1" s="108" t="inlineStr">
+        <is>
+          <t>Customer_Legal_Name</t>
+        </is>
+      </c>
+      <c r="AF1" s="107" t="inlineStr">
+        <is>
+          <t>NoticeStatus</t>
+        </is>
+      </c>
+      <c r="AG1" s="110" t="inlineStr">
+        <is>
+          <t>HostBankSharePct</t>
+        </is>
+      </c>
+      <c r="AH1" s="110" t="inlineStr">
+        <is>
+          <t>LenderSharePct1</t>
+        </is>
+      </c>
+      <c r="AI1" s="110" t="inlineStr">
+        <is>
+          <t>LenderSharePct2</t>
+        </is>
+      </c>
+      <c r="AJ1" s="110" t="inlineStr">
+        <is>
+          <t>Host_Bank</t>
+        </is>
+      </c>
+      <c r="AK1" s="107" t="inlineStr">
+        <is>
+          <t>Rollover_Amount</t>
+        </is>
+      </c>
+      <c r="AL1" s="107" t="inlineStr">
+        <is>
+          <t>Repricing_Frequency</t>
+        </is>
+      </c>
+      <c r="AM1" s="13" t="inlineStr">
+        <is>
+          <t>Loan_EffectiveDate</t>
+        </is>
+      </c>
+      <c r="AN1" s="43" t="inlineStr">
+        <is>
+          <t>Loan_TotalGlobalInterest</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" s="93" t="inlineStr">
+        <is>
+          <t>EVG_S1_EU_RPA_InternalDeal</t>
+        </is>
+      </c>
+      <c r="C2" s="116" t="inlineStr">
+        <is>
+          <t>RPA INTERNAL 100M EURO04112020090259OJX</t>
+        </is>
+      </c>
+      <c r="D2" s="111" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="E2" s="105" t="inlineStr">
+        <is>
+          <t>INTFULDRAW04112020091041ZVV</t>
+        </is>
+      </c>
+      <c r="F2" s="106" t="inlineStr">
+        <is>
+          <t>60000715</t>
+        </is>
+      </c>
+      <c r="G2" s="111" t="inlineStr">
+        <is>
+          <t>Comprehensive Repricing</t>
+        </is>
+      </c>
+      <c r="H2" s="117" t="inlineStr">
+        <is>
+          <t>19-Jun-2018</t>
+        </is>
+      </c>
+      <c r="I2" s="118" t="inlineStr">
+        <is>
+          <t>Principal Payment</t>
+        </is>
+      </c>
+      <c r="J2" s="118" t="inlineStr">
+        <is>
+          <t>Rollover/Conversion to New:</t>
+        </is>
+      </c>
+      <c r="K2" s="118" t="inlineStr">
+        <is>
+          <t>Euro LIBOR Option</t>
+        </is>
+      </c>
+      <c r="L2" s="93" t="inlineStr">
+        <is>
+          <t>SHORTNME2255</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>COMMONWEALTH BANK AU-OBU</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>CBA AMSTERDAM</t>
+        </is>
+      </c>
+      <c r="O2" s="118" t="inlineStr">
+        <is>
+          <t>IMT</t>
+        </is>
+      </c>
+      <c r="P2" s="118" t="inlineStr">
+        <is>
+          <t>IMT</t>
+        </is>
+      </c>
+      <c r="Q2" s="118" t="inlineStr">
+        <is>
+          <t>IMT</t>
+        </is>
+      </c>
+      <c r="R2" s="118" t="inlineStr">
+        <is>
+          <t>IMT</t>
+        </is>
+      </c>
+      <c r="S2" s="118" t="inlineStr">
+        <is>
+          <t>IMT</t>
+        </is>
+      </c>
+      <c r="T2" s="118" t="inlineStr">
+        <is>
+          <t>IMT</t>
+        </is>
+      </c>
+      <c r="U2" t="n">
+        <v>40000000</v>
+      </c>
+      <c r="V2" s="5" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="W2" s="5" t="inlineStr">
+        <is>
+          <t>Approved</t>
+        </is>
+      </c>
+      <c r="X2" s="114" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="Y2" s="119" t="inlineStr">
+        <is>
+          <t>JCUSR01</t>
+        </is>
+      </c>
+      <c r="Z2" s="120" t="inlineStr">
+        <is>
+          <t>password</t>
+        </is>
+      </c>
+      <c r="AA2" s="119" t="inlineStr">
+        <is>
+          <t>JCAPR01</t>
+        </is>
+      </c>
+      <c r="AB2" s="119" t="inlineStr">
+        <is>
+          <t>password</t>
+        </is>
+      </c>
+      <c r="AC2" s="119" t="inlineStr">
+        <is>
+          <t>JCAPR02</t>
+        </is>
+      </c>
+      <c r="AD2" s="119" t="inlineStr">
+        <is>
+          <t>password</t>
+        </is>
+      </c>
+      <c r="AF2" s="5" t="inlineStr">
+        <is>
+          <t>Awaiting release</t>
+        </is>
+      </c>
+      <c r="AG2" t="n">
+        <v>100</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>50</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>50</v>
+      </c>
+      <c r="AJ2" t="inlineStr">
+        <is>
+          <t>CB001/Hold for Investment - Australia/012689</t>
+        </is>
+      </c>
+      <c r="AK2" s="113" t="n">
+        <v>40000000</v>
+      </c>
+      <c r="AL2" t="inlineStr">
+        <is>
+          <t>1 Months</t>
+        </is>
+      </c>
+      <c r="AM2" s="52" t="inlineStr">
+        <is>
+          <t>10-Aug-2020</t>
+        </is>
+      </c>
+      <c r="AN2" s="115" t="n">
+        <v>520833.33</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" s="93" t="inlineStr">
+        <is>
+          <t>EVG_S1_EU_RPA_InternalDeal</t>
+        </is>
+      </c>
+      <c r="C3" s="104" t="inlineStr">
+        <is>
+          <t>RPA INTERNAL 100M EURO04112020090259OJX</t>
+        </is>
+      </c>
+      <c r="D3" s="111" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="E3" s="105" t="inlineStr">
+        <is>
+          <t>PARDRAW04112020091859TQL</t>
+        </is>
+      </c>
+      <c r="F3" s="105" t="inlineStr">
+        <is>
+          <t>60000716</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B4" s="93" t="inlineStr">
+        <is>
+          <t>EVG_S1_EU_RPA_InternalDeal</t>
+        </is>
+      </c>
+      <c r="C4" s="104" t="inlineStr">
+        <is>
+          <t>RPA INTERNAL 100M EURO04112020090259OJX</t>
+        </is>
+      </c>
+      <c r="E4" s="105" t="inlineStr">
+        <is>
+          <t>INTUND04112020092726MHD</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:AP2"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -3165,7 +3707,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -3256,17 +3798,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CW4"/>
+  <dimension ref="A1:CV4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="W1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AC2" sqref="AC2"/>
+      <pane xSplit="2" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S1" sqref="S1:S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -3292,83 +3834,82 @@
     <col width="18.7109375" customWidth="1" style="93" min="19" max="19"/>
     <col width="14.42578125" customWidth="1" style="93" min="20" max="20"/>
     <col width="20.5703125" customWidth="1" style="93" min="21" max="22"/>
-    <col width="17.7109375" customWidth="1" style="93" min="23" max="23"/>
-    <col width="13.85546875" customWidth="1" style="93" min="24" max="24"/>
-    <col width="21" customWidth="1" style="93" min="25" max="25"/>
-    <col width="13.140625" customWidth="1" style="93" min="26" max="26"/>
-    <col width="19.28515625" customWidth="1" style="93" min="27" max="27"/>
-    <col width="18" customWidth="1" style="15" min="28" max="28"/>
-    <col width="40.85546875" customWidth="1" style="15" min="29" max="29"/>
-    <col width="24.42578125" customWidth="1" style="93" min="30" max="30"/>
-    <col width="30.42578125" customWidth="1" style="93" min="31" max="31"/>
-    <col width="36" customWidth="1" style="93" min="32" max="32"/>
-    <col width="34.42578125" customWidth="1" style="93" min="33" max="33"/>
-    <col width="26.7109375" customWidth="1" style="93" min="34" max="34"/>
-    <col width="17.28515625" customWidth="1" style="93" min="35" max="36"/>
-    <col width="34.140625" customWidth="1" style="93" min="37" max="37"/>
-    <col width="28.42578125" customWidth="1" style="93" min="38" max="38"/>
-    <col width="24.7109375" customWidth="1" style="93" min="39" max="39"/>
-    <col width="30.28515625" customWidth="1" style="93" min="40" max="40"/>
-    <col width="17.5703125" customWidth="1" style="93" min="41" max="41"/>
-    <col width="20.28515625" customWidth="1" style="93" min="42" max="42"/>
-    <col width="12.140625" customWidth="1" style="93" min="43" max="43"/>
-    <col width="21.42578125" customWidth="1" style="93" min="44" max="44"/>
-    <col width="24.140625" customWidth="1" style="93" min="45" max="45"/>
-    <col width="16" customWidth="1" style="93" min="46" max="46"/>
-    <col width="14" customWidth="1" style="93" min="47" max="47"/>
-    <col width="16.7109375" customWidth="1" style="93" min="48" max="48"/>
-    <col width="10" customWidth="1" style="93" min="49" max="49"/>
-    <col width="8.5703125" customWidth="1" style="93" min="50" max="50"/>
-    <col width="19.140625" customWidth="1" style="93" min="51" max="51"/>
-    <col width="37.7109375" customWidth="1" style="93" min="52" max="52"/>
-    <col width="15.85546875" customWidth="1" style="93" min="53" max="53"/>
-    <col width="9.28515625" customWidth="1" style="93" min="54" max="54"/>
-    <col width="16.7109375" customWidth="1" style="93" min="55" max="56"/>
-    <col width="12.85546875" customWidth="1" style="93" min="57" max="57"/>
-    <col width="32.42578125" customWidth="1" style="93" min="58" max="58"/>
-    <col width="11.7109375" customWidth="1" style="93" min="59" max="59"/>
-    <col width="35" customWidth="1" style="93" min="60" max="60"/>
-    <col width="18.140625" customWidth="1" style="93" min="61" max="61"/>
-    <col width="15.7109375" customWidth="1" style="93" min="62" max="62"/>
-    <col width="24" customWidth="1" style="93" min="63" max="63"/>
-    <col width="11.5703125" customWidth="1" style="93" min="64" max="64"/>
-    <col width="8.28515625" customWidth="1" style="93" min="65" max="65"/>
-    <col width="16.5703125" customWidth="1" style="93" min="66" max="66"/>
-    <col width="32.85546875" customWidth="1" style="93" min="67" max="67"/>
-    <col width="18.7109375" customWidth="1" style="93" min="68" max="68"/>
-    <col width="18.28515625" customWidth="1" style="93" min="69" max="69"/>
-    <col width="10.42578125" customWidth="1" style="93" min="70" max="70"/>
-    <col width="9.7109375" customWidth="1" style="93" min="71" max="71"/>
-    <col width="12.7109375" customWidth="1" style="93" min="72" max="72"/>
-    <col width="11.7109375" customWidth="1" style="93" min="73" max="73"/>
-    <col width="24" customWidth="1" style="93" min="74" max="74"/>
-    <col width="43.7109375" customWidth="1" style="93" min="75" max="75"/>
-    <col width="44.85546875" customWidth="1" style="93" min="76" max="76"/>
-    <col width="30.140625" customWidth="1" style="93" min="77" max="77"/>
-    <col width="29.42578125" customWidth="1" style="93" min="78" max="78"/>
-    <col width="25.28515625" customWidth="1" style="93" min="79" max="79"/>
-    <col width="9.5703125" customWidth="1" style="93" min="80" max="80"/>
-    <col width="25.7109375" customWidth="1" style="93" min="81" max="81"/>
-    <col width="19.7109375" customWidth="1" style="93" min="82" max="82"/>
-    <col width="28.5703125" customWidth="1" style="93" min="83" max="83"/>
-    <col width="21.140625" customWidth="1" style="93" min="84" max="84"/>
-    <col width="14.5703125" customWidth="1" style="93" min="85" max="85"/>
-    <col width="20.5703125" customWidth="1" style="93" min="86" max="86"/>
-    <col width="18.28515625" customWidth="1" style="93" min="87" max="87"/>
-    <col width="18.85546875" customWidth="1" style="93" min="88" max="88"/>
-    <col width="35" customWidth="1" style="93" min="89" max="89"/>
-    <col width="20" customWidth="1" style="93" min="90" max="90"/>
-    <col width="32.42578125" customWidth="1" style="93" min="91" max="91"/>
-    <col width="21.5703125" customWidth="1" style="93" min="92" max="92"/>
-    <col width="13.5703125" customWidth="1" style="93" min="93" max="93"/>
-    <col width="26.28515625" customWidth="1" style="93" min="94" max="94"/>
-    <col width="19.140625" customWidth="1" style="93" min="95" max="95"/>
-    <col width="44" customWidth="1" style="93" min="96" max="96"/>
-    <col width="23.5703125" customWidth="1" style="93" min="97" max="97"/>
-    <col width="26.28515625" customWidth="1" style="93" min="98" max="98"/>
-    <col width="34.85546875" customWidth="1" style="93" min="99" max="99"/>
-    <col width="9.140625" customWidth="1" style="93" min="100" max="100"/>
-    <col width="15.85546875" customWidth="1" style="93" min="101" max="101"/>
+    <col width="13.85546875" customWidth="1" style="93" min="23" max="23"/>
+    <col width="21" customWidth="1" style="93" min="24" max="24"/>
+    <col width="13.140625" customWidth="1" style="93" min="25" max="25"/>
+    <col width="19.28515625" customWidth="1" style="93" min="26" max="26"/>
+    <col width="18" customWidth="1" style="15" min="27" max="27"/>
+    <col width="40.85546875" customWidth="1" style="15" min="28" max="28"/>
+    <col width="24.42578125" customWidth="1" style="93" min="29" max="29"/>
+    <col width="30.42578125" customWidth="1" style="93" min="30" max="30"/>
+    <col width="36" customWidth="1" style="93" min="31" max="31"/>
+    <col width="34.42578125" customWidth="1" style="93" min="32" max="32"/>
+    <col width="26.7109375" customWidth="1" style="93" min="33" max="33"/>
+    <col width="17.28515625" customWidth="1" style="93" min="34" max="35"/>
+    <col width="34.140625" customWidth="1" style="93" min="36" max="36"/>
+    <col width="28.42578125" customWidth="1" style="93" min="37" max="37"/>
+    <col width="24.7109375" customWidth="1" style="93" min="38" max="38"/>
+    <col width="30.28515625" customWidth="1" style="93" min="39" max="39"/>
+    <col width="17.5703125" customWidth="1" style="93" min="40" max="40"/>
+    <col width="20.28515625" customWidth="1" style="93" min="41" max="41"/>
+    <col width="12.140625" customWidth="1" style="93" min="42" max="42"/>
+    <col width="21.42578125" customWidth="1" style="93" min="43" max="43"/>
+    <col width="24.140625" customWidth="1" style="93" min="44" max="44"/>
+    <col width="16" customWidth="1" style="93" min="45" max="45"/>
+    <col width="14" customWidth="1" style="93" min="46" max="46"/>
+    <col width="16.7109375" customWidth="1" style="93" min="47" max="47"/>
+    <col width="10" customWidth="1" style="93" min="48" max="48"/>
+    <col width="8.5703125" customWidth="1" style="93" min="49" max="49"/>
+    <col width="19.140625" customWidth="1" style="93" min="50" max="50"/>
+    <col width="37.7109375" customWidth="1" style="93" min="51" max="51"/>
+    <col width="15.85546875" customWidth="1" style="93" min="52" max="52"/>
+    <col width="9.28515625" customWidth="1" style="93" min="53" max="53"/>
+    <col width="16.7109375" customWidth="1" style="93" min="54" max="55"/>
+    <col width="12.85546875" customWidth="1" style="93" min="56" max="56"/>
+    <col width="32.42578125" customWidth="1" style="93" min="57" max="57"/>
+    <col width="11.7109375" customWidth="1" style="93" min="58" max="58"/>
+    <col width="35" customWidth="1" style="93" min="59" max="59"/>
+    <col width="18.140625" customWidth="1" style="93" min="60" max="60"/>
+    <col width="15.7109375" customWidth="1" style="93" min="61" max="61"/>
+    <col width="24" customWidth="1" style="93" min="62" max="62"/>
+    <col width="11.5703125" customWidth="1" style="93" min="63" max="63"/>
+    <col width="8.28515625" customWidth="1" style="93" min="64" max="64"/>
+    <col width="16.5703125" customWidth="1" style="93" min="65" max="65"/>
+    <col width="32.85546875" customWidth="1" style="93" min="66" max="66"/>
+    <col width="18.7109375" customWidth="1" style="93" min="67" max="67"/>
+    <col width="18.28515625" customWidth="1" style="93" min="68" max="68"/>
+    <col width="10.42578125" customWidth="1" style="93" min="69" max="69"/>
+    <col width="9.7109375" customWidth="1" style="93" min="70" max="70"/>
+    <col width="12.7109375" customWidth="1" style="93" min="71" max="71"/>
+    <col width="11.7109375" customWidth="1" style="93" min="72" max="72"/>
+    <col width="24" customWidth="1" style="93" min="73" max="73"/>
+    <col width="43.7109375" customWidth="1" style="93" min="74" max="74"/>
+    <col width="44.85546875" customWidth="1" style="93" min="75" max="75"/>
+    <col width="30.140625" customWidth="1" style="93" min="76" max="76"/>
+    <col width="29.42578125" customWidth="1" style="93" min="77" max="77"/>
+    <col width="25.28515625" customWidth="1" style="93" min="78" max="78"/>
+    <col width="9.5703125" customWidth="1" style="93" min="79" max="79"/>
+    <col width="25.7109375" customWidth="1" style="93" min="80" max="80"/>
+    <col width="19.7109375" customWidth="1" style="93" min="81" max="81"/>
+    <col width="28.5703125" customWidth="1" style="93" min="82" max="82"/>
+    <col width="21.140625" customWidth="1" style="93" min="83" max="83"/>
+    <col width="14.5703125" customWidth="1" style="93" min="84" max="84"/>
+    <col width="20.5703125" customWidth="1" style="93" min="85" max="85"/>
+    <col width="18.28515625" customWidth="1" style="93" min="86" max="86"/>
+    <col width="18.85546875" customWidth="1" style="93" min="87" max="87"/>
+    <col width="35" customWidth="1" style="93" min="88" max="88"/>
+    <col width="20" customWidth="1" style="93" min="89" max="89"/>
+    <col width="32.42578125" customWidth="1" style="93" min="90" max="90"/>
+    <col width="21.5703125" customWidth="1" style="93" min="91" max="91"/>
+    <col width="13.5703125" customWidth="1" style="93" min="92" max="92"/>
+    <col width="26.28515625" customWidth="1" style="93" min="93" max="93"/>
+    <col width="19.140625" customWidth="1" style="93" min="94" max="94"/>
+    <col width="44" customWidth="1" style="93" min="95" max="95"/>
+    <col width="23.5703125" customWidth="1" style="93" min="96" max="96"/>
+    <col width="26.28515625" customWidth="1" style="93" min="97" max="97"/>
+    <col width="34.85546875" customWidth="1" style="93" min="98" max="98"/>
+    <col width="9.140625" customWidth="1" style="93" min="99" max="99"/>
+    <col width="15.85546875" customWidth="1" style="93" min="100" max="100"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customFormat="1" customHeight="1" s="1">
@@ -3482,41 +4023,37 @@
           <t>HostBank_GLAccount</t>
         </is>
       </c>
-      <c r="W1" s="13" t="inlineStr">
-        <is>
-          <t>LoanEffectiveDate</t>
+      <c r="W1" s="2" t="inlineStr">
+        <is>
+          <t>ActualAmount</t>
         </is>
       </c>
       <c r="X1" s="2" t="inlineStr">
         <is>
-          <t>ActualAmount</t>
+          <t>Facility_ProposedCmt</t>
         </is>
       </c>
       <c r="Y1" s="2" t="inlineStr">
         <is>
-          <t>Facility_ProposedCmt</t>
+          <t>Facility_Type</t>
         </is>
       </c>
       <c r="Z1" s="2" t="inlineStr">
         <is>
-          <t>Facility_Type</t>
-        </is>
-      </c>
-      <c r="AA1" s="2" t="inlineStr">
-        <is>
           <t>Contact_Email</t>
         </is>
       </c>
+      <c r="AA1" s="13" t="inlineStr">
+        <is>
+          <t>HostBankSharePct</t>
+        </is>
+      </c>
       <c r="AB1" s="13" t="inlineStr">
         <is>
-          <t>HostBankSharePct</t>
-        </is>
-      </c>
-      <c r="AC1" s="13" t="inlineStr">
-        <is>
           <t>Host_Bank</t>
         </is>
       </c>
+      <c r="AW1" s="36" t="n"/>
       <c r="AX1" s="36" t="n"/>
       <c r="AY1" s="36" t="n"/>
       <c r="AZ1" s="36" t="n"/>
@@ -3568,7 +4105,6 @@
       <c r="CT1" s="36" t="n"/>
       <c r="CU1" s="36" t="n"/>
       <c r="CV1" s="36" t="n"/>
-      <c r="CW1" s="36" t="n"/>
     </row>
     <row r="2" ht="12.75" customFormat="1" customHeight="1" s="93">
       <c r="A2" s="93" t="inlineStr">
@@ -3613,7 +4149,7 @@
       </c>
       <c r="I2" s="93" t="inlineStr">
         <is>
-          <t>60000481</t>
+          <t>60000639</t>
         </is>
       </c>
       <c r="J2" s="93" t="inlineStr">
@@ -3661,9 +4197,9 @@
           <t>1</t>
         </is>
       </c>
-      <c r="S2" s="93" t="inlineStr">
-        <is>
-          <t>22-May-2020</t>
+      <c r="S2" s="52" t="inlineStr">
+        <is>
+          <t>10-Aug-2020</t>
         </is>
       </c>
       <c r="U2" s="93" t="inlineStr">
@@ -3678,33 +4214,28 @@
       </c>
       <c r="W2" s="93" t="inlineStr">
         <is>
-          <t>22-May-2020</t>
+          <t>833.33</t>
         </is>
       </c>
       <c r="X2" s="93" t="inlineStr">
         <is>
-          <t>833.33</t>
+          <t>100,000.00</t>
         </is>
       </c>
       <c r="Y2" s="93" t="inlineStr">
         <is>
-          <t>100,000.00</t>
-        </is>
-      </c>
-      <c r="Z2" s="93" t="inlineStr">
-        <is>
           <t>Term</t>
         </is>
       </c>
-      <c r="AA2" s="31" t="inlineStr">
+      <c r="Z2" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">john.blogg@abc.com </t>
         </is>
       </c>
-      <c r="AB2" s="32" t="n">
+      <c r="AA2" s="32" t="n">
         <v>100</v>
       </c>
-      <c r="AC2" s="93" t="inlineStr">
+      <c r="AB2" s="93" t="inlineStr">
         <is>
           <t>CB001/Hold for Investment - Australia/BP_CML</t>
         </is>
@@ -3731,7 +4262,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -3739,8 +4270,8 @@
   </sheetPr>
   <dimension ref="A1:AT4"/>
   <sheetViews>
-    <sheetView topLeftCell="AO1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AT2" sqref="AT2"/>
+    <sheetView topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -4066,12 +4597,12 @@
       </c>
       <c r="I2" s="93" t="inlineStr">
         <is>
-          <t>60000481</t>
+          <t>60000639</t>
         </is>
       </c>
       <c r="K2" s="93" t="inlineStr">
         <is>
-          <t>22-Jun-2020</t>
+          <t>03-Dec-2020</t>
         </is>
       </c>
       <c r="L2" s="15" t="inlineStr">
@@ -4244,6 +4775,11 @@
       <c r="A3" s="93" t="inlineStr">
         <is>
           <t>2</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>03-Dec-2020</t>
         </is>
       </c>
     </row>
@@ -4262,7 +4798,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -4271,8 +4807,8 @@
   <dimension ref="A1:AL5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N2" sqref="N2"/>
+      <pane xSplit="2" topLeftCell="Y1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AC1" sqref="AC1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -4541,7 +5077,7 @@
       </c>
       <c r="G2" s="93" t="inlineStr">
         <is>
-          <t>RPA INTERNAL 100M EURO30102020121245TGJ</t>
+          <t>RPA INTERNAL 100M EURO04112020090259OJX</t>
         </is>
       </c>
       <c r="I2" s="93" t="inlineStr">
@@ -4596,7 +5132,7 @@
       </c>
       <c r="S2" s="93" t="inlineStr">
         <is>
-          <t>RPA INTERNAL 100M EURO30102020121245TGJ</t>
+          <t>RPA INTERNAL 100M EURO04112020090259OJX</t>
         </is>
       </c>
       <c r="T2" s="93" t="inlineStr">
@@ -4611,17 +5147,17 @@
       </c>
       <c r="V2" s="93" t="inlineStr">
         <is>
-          <t>10-Aug-2020</t>
+          <t>03-Nov-2020</t>
         </is>
       </c>
       <c r="W2" s="93" t="inlineStr">
         <is>
-          <t>10-Aug-2020</t>
+          <t>03-Nov-2020</t>
         </is>
       </c>
       <c r="X2" s="93" t="inlineStr">
         <is>
-          <t>10-Aug-2020</t>
+          <t>03-Nov-2020</t>
         </is>
       </c>
       <c r="Y2" s="93" t="inlineStr">
@@ -4717,7 +5253,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -4817,10 +5353,10 @@
   <dimension ref="A1:AQ8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="A1" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
-      <selection pane="bottomRight" activeCell="AC2" sqref="AC2"/>
+      <selection pane="bottomRight" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4862,8 +5398,8 @@
     <col width="8.7109375" customWidth="1" style="64" min="42" max="42"/>
     <col width="11.28515625" customWidth="1" style="64" min="43" max="43"/>
     <col width="8.7109375" customWidth="1" style="64" min="44" max="45"/>
-    <col width="9.140625" customWidth="1" style="68" min="46" max="90"/>
-    <col width="9.140625" customWidth="1" style="68" min="91" max="16384"/>
+    <col width="9.140625" customWidth="1" style="68" min="46" max="96"/>
+    <col width="9.140625" customWidth="1" style="68" min="97" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customFormat="1" customHeight="1" s="61">
@@ -7554,9 +8090,9 @@
   </sheetPr>
   <dimension ref="A1:CY4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="BJ1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BP1" sqref="BP1"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="AB1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AB11" sqref="AB11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -8199,17 +8735,17 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>RPA INTERNAL 100M EURO30102020121245TGJ</t>
+          <t>RPA INTERNAL 100M EURO04112020090259OJX</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>R1_30102020121248TXD</t>
+          <t>R1_04112020090301SEW</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>INTFULDRAW30102020122129DGS</t>
+          <t>INTFULDRAW04112020091041ZVV</t>
         </is>
       </c>
       <c r="H2" s="93" t="inlineStr">
@@ -8329,7 +8865,7 @@
       </c>
       <c r="AE2" s="48" t="inlineStr">
         <is>
-          <t>10-Aug-2020</t>
+          <t>03-Nov-2020</t>
         </is>
       </c>
       <c r="AF2" s="48" t="n"/>
@@ -8433,17 +8969,17 @@
       </c>
       <c r="BJ2" t="inlineStr">
         <is>
-          <t>10-Aug-2020</t>
+          <t>03-Nov-2020</t>
         </is>
       </c>
       <c r="BL2" t="inlineStr">
         <is>
-          <t>10-Aug-2020</t>
+          <t>03-Nov-2020</t>
         </is>
       </c>
       <c r="BN2" t="inlineStr">
         <is>
-          <t>10-Aug-2020</t>
+          <t>03-Nov-2020</t>
         </is>
       </c>
       <c r="BO2" s="48" t="n"/>
@@ -8479,17 +9015,17 @@
       </c>
       <c r="CJ2" t="inlineStr">
         <is>
-          <t>10-Aug-2020</t>
+          <t>03-Nov-2020</t>
         </is>
       </c>
       <c r="CK2" t="inlineStr">
         <is>
-          <t>10-Aug-2020</t>
+          <t>03-Nov-2020</t>
         </is>
       </c>
       <c r="CM2" t="inlineStr">
         <is>
-          <t>10-Aug-2020</t>
+          <t>03-Nov-2020</t>
         </is>
       </c>
       <c r="CN2" s="14" t="inlineStr">
@@ -8554,17 +9090,17 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>RPA INTERNAL 100M EURO30102020121245TGJ</t>
+          <t>RPA INTERNAL 100M EURO04112020090259OJX</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>R1_30102020121248TXD</t>
+          <t>R1_04112020090301SEW</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>PARDRAW30102020123027LKM</t>
+          <t>PARDRAW04112020091859TQL</t>
         </is>
       </c>
       <c r="H3" s="93" t="inlineStr">
@@ -8909,17 +9445,17 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>RPA INTERNAL 100M EURO30102020121245TGJ</t>
+          <t>RPA INTERNAL 100M EURO04112020090259OJX</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>R1_30102020121248TXD</t>
+          <t>R1_04112020090301SEW</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>INTUND30102020123930CUQ</t>
+          <t>INTUND04112020092726MHD</t>
         </is>
       </c>
       <c r="H4" s="93" t="inlineStr">
@@ -9258,8 +9794,8 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G9" sqref="G9"/>
+      <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -9338,9 +9874,9 @@
           <t>EVG_S1_EU_RPA_InternalDeal</t>
         </is>
       </c>
-      <c r="C2" s="92" t="inlineStr">
-        <is>
-          <t>RPA INTERNAL 100M EURO30102020121245TGJ</t>
+      <c r="C2" s="116" t="inlineStr">
+        <is>
+          <t>RPA INTERNAL 100M EURO04112020090259OJX</t>
         </is>
       </c>
       <c r="D2" s="22" t="inlineStr">
@@ -9390,8 +9926,8 @@
   </sheetPr>
   <dimension ref="A1:AX2"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -9710,14 +10246,14 @@
           <t>EVG_S1_EU_RPA_InternalDeal</t>
         </is>
       </c>
-      <c r="C2" s="92" t="inlineStr">
-        <is>
-          <t>RPA INTERNAL 100M EURO30102020121245TGJ</t>
+      <c r="C2" s="116" t="inlineStr">
+        <is>
+          <t>RPA INTERNAL 100M EURO04112020090259OJX</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>INTFULDRAW30102020122129DGS</t>
+          <t>INTFULDRAW04112020091041ZVV</t>
         </is>
       </c>
       <c r="E2" s="93" t="inlineStr">
@@ -9947,10 +10483,10 @@
   <dimension ref="A1:AF4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="A1" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
-      <selection pane="bottomRight" activeCell="H27" sqref="H27"/>
+      <selection pane="bottomRight" activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -10172,12 +10708,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>RPA INTERNAL 100M EURO30102020121245TGJ</t>
+          <t>RPA INTERNAL 100M EURO04112020090259OJX</t>
         </is>
       </c>
       <c r="F2" s="93" t="inlineStr">
         <is>
-          <t>INTFULDRAW30102020122129DGS</t>
+          <t>INTFULDRAW04112020091041ZVV</t>
         </is>
       </c>
       <c r="H2" s="93" t="inlineStr">
@@ -10202,22 +10738,22 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>10-Aug-2020</t>
+          <t>03-Nov-2020</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>10-Aug-2020</t>
+          <t>03-Nov-2020</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>11-Aug-2025</t>
+          <t>03-Nov-2025</t>
         </is>
       </c>
       <c r="P2" s="3" t="inlineStr">
         <is>
-          <t>11-Aug-2025</t>
+          <t>03-Nov-2025</t>
         </is>
       </c>
       <c r="R2" s="93" t="inlineStr">
@@ -10309,12 +10845,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>RPA INTERNAL 100M EURO30102020121245TGJ</t>
+          <t>RPA INTERNAL 100M EURO04112020090259OJX</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>PARDRAW30102020123027LKM</t>
+          <t>PARDRAW04112020091859TQL</t>
         </is>
       </c>
       <c r="H3" s="93" t="inlineStr">
@@ -10339,22 +10875,22 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>10-Aug-2020</t>
+          <t>03-Nov-2020</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>10-Aug-2020</t>
+          <t>03-Nov-2020</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>11-Aug-2025</t>
+          <t>03-Nov-2025</t>
         </is>
       </c>
       <c r="P3" s="3" t="inlineStr">
         <is>
-          <t>11-Aug-2025</t>
+          <t>03-Nov-2025</t>
         </is>
       </c>
       <c r="R3" s="93" t="inlineStr">
@@ -10446,12 +10982,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>RPA INTERNAL 100M EURO30102020121245TGJ</t>
+          <t>RPA INTERNAL 100M EURO04112020090259OJX</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>INTUND30102020123930CUQ</t>
+          <t>INTUND04112020092726MHD</t>
         </is>
       </c>
       <c r="H4" s="93" t="inlineStr">
@@ -10476,22 +11012,22 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>10-Aug-2020</t>
+          <t>03-Nov-2020</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>10-Aug-2020</t>
+          <t>03-Nov-2020</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>11-Aug-2025</t>
+          <t>03-Nov-2025</t>
         </is>
       </c>
       <c r="P4" s="3" t="inlineStr">
         <is>
-          <t>11-Aug-2025</t>
+          <t>03-Nov-2025</t>
         </is>
       </c>
       <c r="R4" s="93" t="inlineStr">
@@ -10577,10 +11113,10 @@
   <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="A1" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
-      <selection pane="bottomRight" activeCell="P17" sqref="P17"/>
+      <selection pane="bottomRight" activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -10725,7 +11261,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>INTFULDRAW30102020122129DGS</t>
+          <t>INTFULDRAW04112020091041ZVV</t>
         </is>
       </c>
       <c r="D2" s="22" t="inlineStr">
@@ -10832,7 +11368,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>PARDRAW30102020123027LKM</t>
+          <t>PARDRAW04112020091859TQL</t>
         </is>
       </c>
       <c r="D3" s="22" t="inlineStr">
@@ -10939,7 +11475,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>INTUND30102020123930CUQ</t>
+          <t>INTUND04112020092726MHD</t>
         </is>
       </c>
       <c r="D4" s="22" t="inlineStr">
@@ -11246,12 +11782,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>RPA INTERNAL 100M EURO30102020121245TGJ</t>
+          <t>RPA INTERNAL 100M EURO04112020090259OJX</t>
         </is>
       </c>
       <c r="D2" s="93" t="inlineStr">
         <is>
-          <t>INTFULDRAW30102020122129DGS</t>
+          <t>INTFULDRAW04112020091041ZVV</t>
         </is>
       </c>
       <c r="E2" s="93" t="inlineStr">
@@ -11327,12 +11863,12 @@
       </c>
       <c r="T2" s="93" t="inlineStr">
         <is>
-          <t>11-Aug-2025</t>
+          <t>03-Nov-2025</t>
         </is>
       </c>
       <c r="U2" s="93" t="inlineStr">
         <is>
-          <t>10-Aug-2020</t>
+          <t>03-Nov-2020</t>
         </is>
       </c>
       <c r="W2" s="93" t="inlineStr">
@@ -11347,12 +11883,12 @@
       </c>
       <c r="Y2" s="93" t="inlineStr">
         <is>
-          <t>10-Aug-2020</t>
+          <t>03-Nov-2020</t>
         </is>
       </c>
       <c r="Z2" s="93" t="inlineStr">
         <is>
-          <t>10-Aug-2020</t>
+          <t>03-Nov-2020</t>
         </is>
       </c>
       <c r="AA2" s="93" t="inlineStr">
@@ -11384,12 +11920,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>RPA INTERNAL 100M EURO30102020121245TGJ</t>
+          <t>RPA INTERNAL 100M EURO04112020090259OJX</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>PARDRAW30102020123027LKM</t>
+          <t>PARDRAW04112020091859TQL</t>
         </is>
       </c>
       <c r="E3" s="93" t="inlineStr">
@@ -11465,7 +12001,7 @@
       </c>
       <c r="T3" s="93" t="inlineStr">
         <is>
-          <t>11-Aug-2025</t>
+          <t>03-Nov-2025</t>
         </is>
       </c>
       <c r="U3" s="93" t="inlineStr">
@@ -11522,12 +12058,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>RPA INTERNAL 100M EURO30102020121245TGJ</t>
+          <t>RPA INTERNAL 100M EURO04112020090259OJX</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>INTUND30102020123930CUQ</t>
+          <t>INTUND04112020092726MHD</t>
         </is>
       </c>
       <c r="E4" s="93" t="inlineStr">
@@ -11603,7 +12139,7 @@
       </c>
       <c r="T4" s="93" t="inlineStr">
         <is>
-          <t>11-Aug-2025</t>
+          <t>03-Nov-2025</t>
         </is>
       </c>
       <c r="U4" s="93" t="inlineStr">

</xml_diff>